<commit_message>
Accept Asia as a region value
The current benchmark data treats Asia as "Global" but that doesn't mean we cannot properly list Asia as a distinct region for display and aggregation purposes.  Accordingly, change POSCO's region to Asia.
</commit_message>
<xml_diff>
--- a/examples/data/20220215 ITR Tool Sample Data.xlsx
+++ b/examples/data/20220215 ITR Tool Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CB7038-EE6D-4048-8871-60B1276B9695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C41D903-EF1B-7840-BD20-10599860FD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45940" yWindow="2320" windowWidth="48600" windowHeight="39960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45940" yWindow="2320" windowWidth="48600" windowHeight="39960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -424,7 +424,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="324">
   <si>
     <t>Data field</t>
   </si>
@@ -1519,6 +1519,9 @@
   </si>
   <si>
     <t>investment_value</t>
+  </si>
+  <si>
+    <t>Asia</t>
   </si>
 </sst>
 </file>
@@ -3279,11 +3282,11 @@
   </sheetPr>
   <dimension ref="A1:AZ50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U16" sqref="U16"/>
+      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -6742,7 +6745,7 @@
         <v>260</v>
       </c>
       <c r="E32" s="61" t="s">
-        <v>227</v>
+        <v>323</v>
       </c>
       <c r="F32" s="61" t="s">
         <v>182</v>
@@ -7300,11 +7303,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AEF12C-8FCA-4C98-A7E3-A92507F3829D}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L22" sqref="L22"/>
+      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10094,7 +10097,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>166892</v>
+        <v>152437</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -10112,7 +10115,7 @@
       </c>
       <c r="E3" s="61">
         <f t="shared" ref="E3:E41" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
-        <v>213623</v>
+        <v>148638</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -10130,7 +10133,7 @@
       </c>
       <c r="E4" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>213332</v>
+        <v>55234</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -10148,7 +10151,7 @@
       </c>
       <c r="E5" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>106708</v>
+        <v>213804</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -10166,7 +10169,7 @@
       </c>
       <c r="E6" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>198499</v>
+        <v>247488</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -10184,7 +10187,7 @@
       </c>
       <c r="E7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>183079</v>
+        <v>180017</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -10202,7 +10205,7 @@
       </c>
       <c r="E8" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>172148</v>
+        <v>185397</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10220,7 +10223,7 @@
       </c>
       <c r="E9" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>35096</v>
+        <v>83634</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -10238,7 +10241,7 @@
       </c>
       <c r="E10" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>83754</v>
+        <v>128256</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -10256,7 +10259,7 @@
       </c>
       <c r="E11" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>162238</v>
+        <v>212093</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -10274,7 +10277,7 @@
       </c>
       <c r="E12" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>198100</v>
+        <v>74230</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -10292,7 +10295,7 @@
       </c>
       <c r="E13" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>125842</v>
+        <v>100348</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -10310,7 +10313,7 @@
       </c>
       <c r="E14" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>60381</v>
+        <v>242344</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -10328,7 +10331,7 @@
       </c>
       <c r="E15" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>217490</v>
+        <v>111055</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -10346,7 +10349,7 @@
       </c>
       <c r="E16" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>108964</v>
+        <v>246941</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -10364,7 +10367,7 @@
       </c>
       <c r="E17" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>144865</v>
+        <v>64432</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -10382,7 +10385,7 @@
       </c>
       <c r="E18" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>249111</v>
+        <v>195763</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -10400,7 +10403,7 @@
       </c>
       <c r="E19" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>238321</v>
+        <v>145254</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -10418,7 +10421,7 @@
       </c>
       <c r="E20" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>125105</v>
+        <v>199830</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -10436,7 +10439,7 @@
       </c>
       <c r="E21" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>140399</v>
+        <v>171357</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -10454,7 +10457,7 @@
       </c>
       <c r="E22" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>220439</v>
+        <v>151154</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -10472,7 +10475,7 @@
       </c>
       <c r="E23" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>198430</v>
+        <v>47084</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -10490,7 +10493,7 @@
       </c>
       <c r="E24" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>111069</v>
+        <v>199197</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -10508,7 +10511,7 @@
       </c>
       <c r="E25" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>160640</v>
+        <v>69695</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -10526,7 +10529,7 @@
       </c>
       <c r="E26" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>43810</v>
+        <v>113293</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -10544,7 +10547,7 @@
       </c>
       <c r="E27" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>134642</v>
+        <v>203918</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -10562,7 +10565,7 @@
       </c>
       <c r="E28" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>107777</v>
+        <v>96110</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -10580,7 +10583,7 @@
       </c>
       <c r="E29" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>225649</v>
+        <v>92736</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -10598,7 +10601,7 @@
       </c>
       <c r="E30" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>93319</v>
+        <v>150894</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -10616,7 +10619,7 @@
       </c>
       <c r="E31" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>64750</v>
+        <v>160303</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -10634,7 +10637,7 @@
       </c>
       <c r="E32" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>63837</v>
+        <v>227092</v>
       </c>
     </row>
     <row r="33" spans="1:5">

</xml_diff>

<commit_message>
Clean up GHG_SCOPE12 confusion
There was long-standing confusion about the meaning of GHG_SCOPE12 (which, when looked at through one functional path, seemed to depend first and only on production values, and when looked at other ways, seemed to represent emissions values).  It was finally determined that this was, indeed, an emissions-based quantity, and the the production value pathway fed a ratio calculation that resolved to a dimensionless quantity (so it could be calculated just as well from emissions).  In any case, these changes principally fix these and some other problems in the way various column names and variable names work and work together.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data/20220215 ITR Tool Sample Data.xlsx
+++ b/examples/data/20220215 ITR Tool Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06498C7C-4F79-9043-9632-181E861AD1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CF4989-38DB-9044-B4FB-524B19360EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44760" yWindow="6520" windowWidth="32540" windowHeight="22440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44760" yWindow="6520" windowWidth="44560" windowHeight="22440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -173,6 +173,138 @@
             <family val="2"/>
           </rPr>
           <t>Test cast for interpolating missing data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{5CE2AC56-DBD4-F44E-8F7A-F2354A542158}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>As of 2016--their last 10-K as a public company.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{E690D3D1-6563-964F-9370-62C106346114}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>calculated from exhibit 99-1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{ACADDAA5-6A0B-2240-80EB-179B5573D605}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Computed from 20-F</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J32" authorId="0" shapeId="0" xr:uid="{BE1A2F56-E041-FF47-8F16-701373C98C67}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Approximate based on market data graphs</t>
         </r>
       </text>
     </comment>
@@ -1569,7 +1701,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1772,6 +1904,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -1908,7 +2046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2082,6 +2220,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3739,11 +3878,11 @@
   </sheetPr>
   <dimension ref="A1:AZ50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AT3" sqref="AT3"/>
+      <selection pane="bottomRight" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -4932,8 +5071,12 @@
       <c r="K11" s="61">
         <v>5829002000</v>
       </c>
-      <c r="L11" s="61"/>
-      <c r="M11" s="61"/>
+      <c r="L11" s="61">
+        <v>1</v>
+      </c>
+      <c r="M11" s="61">
+        <v>1</v>
+      </c>
       <c r="N11" s="61">
         <v>3758771000</v>
       </c>
@@ -5014,7 +5157,7 @@
         <v>5664119.7339246115</v>
       </c>
     </row>
-    <row r="12" spans="1:52">
+    <row r="12" spans="1:52" ht="16">
       <c r="A12" s="61" t="s">
         <v>190</v>
       </c>
@@ -5042,12 +5185,18 @@
       <c r="I12" s="5">
         <v>44196</v>
       </c>
-      <c r="J12" s="61"/>
+      <c r="J12" s="91">
+        <v>3210376042</v>
+      </c>
       <c r="K12" s="61">
         <v>1639605000</v>
       </c>
-      <c r="L12" s="61"/>
-      <c r="M12" s="61"/>
+      <c r="L12" s="61">
+        <v>1</v>
+      </c>
+      <c r="M12" s="61">
+        <v>1</v>
+      </c>
       <c r="N12" s="61">
         <v>7476298000</v>
       </c>
@@ -6036,12 +6185,19 @@
       <c r="I22" s="5">
         <v>44196</v>
       </c>
-      <c r="J22" s="61"/>
+      <c r="J22" s="61">
+        <f>474900000*45</f>
+        <v>21370500000</v>
+      </c>
       <c r="K22" s="61">
         <v>6736467578.2073479</v>
       </c>
-      <c r="L22" s="61"/>
-      <c r="M22" s="61"/>
+      <c r="L22" s="61">
+        <v>1</v>
+      </c>
+      <c r="M22" s="61">
+        <v>1</v>
+      </c>
       <c r="N22" s="61">
         <v>40960299959.761497</v>
       </c>
@@ -6161,12 +6317,19 @@
       <c r="I23" s="5">
         <v>44196</v>
       </c>
-      <c r="J23" s="61"/>
+      <c r="J23" s="61">
+        <f>571900000*16.72*0.2</f>
+        <v>1912433600</v>
+      </c>
       <c r="K23" s="61">
         <v>9835514922.9662342</v>
       </c>
-      <c r="L23" s="61"/>
-      <c r="M23" s="61"/>
+      <c r="L23" s="61">
+        <v>1</v>
+      </c>
+      <c r="M23" s="61">
+        <v>1</v>
+      </c>
       <c r="N23" s="61">
         <v>13397913513.781719</v>
       </c>
@@ -6654,8 +6817,12 @@
       <c r="K27" s="61">
         <v>19393506493.506489</v>
       </c>
-      <c r="L27" s="61"/>
-      <c r="M27" s="61"/>
+      <c r="L27" s="61">
+        <v>1</v>
+      </c>
+      <c r="M27" s="61">
+        <v>1</v>
+      </c>
       <c r="N27" s="61">
         <v>81770129870.129868</v>
       </c>
@@ -6896,8 +7063,12 @@
       <c r="K29" s="61">
         <v>2231600000</v>
       </c>
-      <c r="L29" s="61"/>
-      <c r="M29" s="61"/>
+      <c r="L29" s="61">
+        <v>1</v>
+      </c>
+      <c r="M29" s="61">
+        <v>1</v>
+      </c>
       <c r="N29" s="61">
         <v>11024300000</v>
       </c>
@@ -7217,12 +7388,18 @@
       <c r="I32" s="5">
         <v>44196</v>
       </c>
-      <c r="J32" s="61"/>
+      <c r="J32" s="61">
+        <v>20260000000</v>
+      </c>
       <c r="K32" s="61">
         <v>55955872344.100883</v>
       </c>
-      <c r="L32" s="61"/>
-      <c r="M32" s="61"/>
+      <c r="L32" s="61">
+        <v>1</v>
+      </c>
+      <c r="M32" s="61">
+        <v>1</v>
+      </c>
       <c r="N32" s="61">
         <v>68553124892.036621</v>
       </c>
@@ -7761,11 +7938,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AEF12C-8FCA-4C98-A7E3-A92507F3829D}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10512,7 +10689,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10555,7 +10732,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>45457</v>
+        <v>112482</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -10573,7 +10750,7 @@
       </c>
       <c r="E3" s="61">
         <f t="shared" ref="E3:E41" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
-        <v>46505</v>
+        <v>79808</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -10591,7 +10768,7 @@
       </c>
       <c r="E4" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>179562</v>
+        <v>197683</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -10609,7 +10786,7 @@
       </c>
       <c r="E5" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>158602</v>
+        <v>103668</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -10627,7 +10804,7 @@
       </c>
       <c r="E6" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>90235</v>
+        <v>238242</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -10645,7 +10822,7 @@
       </c>
       <c r="E7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>174422</v>
+        <v>44179</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -10663,7 +10840,7 @@
       </c>
       <c r="E8" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>216180</v>
+        <v>61886</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10681,7 +10858,7 @@
       </c>
       <c r="E9" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>132170</v>
+        <v>115388</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -10699,7 +10876,7 @@
       </c>
       <c r="E10" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>247162</v>
+        <v>166584</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -10717,7 +10894,7 @@
       </c>
       <c r="E11" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>145476</v>
+        <v>128579</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -10735,7 +10912,7 @@
       </c>
       <c r="E12" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>90890</v>
+        <v>107445</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -10753,7 +10930,7 @@
       </c>
       <c r="E13" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>213532</v>
+        <v>51498</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -10771,7 +10948,7 @@
       </c>
       <c r="E14" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>140436</v>
+        <v>174097</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -10789,7 +10966,7 @@
       </c>
       <c r="E15" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>53066</v>
+        <v>244975</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -10807,7 +10984,7 @@
       </c>
       <c r="E16" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>132638</v>
+        <v>63648</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -10825,7 +11002,7 @@
       </c>
       <c r="E17" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>64666</v>
+        <v>130212</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -10843,7 +11020,7 @@
       </c>
       <c r="E18" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>227328</v>
+        <v>140402</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -10861,7 +11038,7 @@
       </c>
       <c r="E19" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>49115</v>
+        <v>102138</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -10879,7 +11056,7 @@
       </c>
       <c r="E20" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>144979</v>
+        <v>167696</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -10897,7 +11074,7 @@
       </c>
       <c r="E21" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>235570</v>
+        <v>167039</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -10915,7 +11092,7 @@
       </c>
       <c r="E22" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>114985</v>
+        <v>67866</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -10933,7 +11110,7 @@
       </c>
       <c r="E23" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>39722</v>
+        <v>229436</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -10951,7 +11128,7 @@
       </c>
       <c r="E24" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>76485</v>
+        <v>239933</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -10969,7 +11146,7 @@
       </c>
       <c r="E25" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>184401</v>
+        <v>148946</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -10987,7 +11164,7 @@
       </c>
       <c r="E26" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>40859</v>
+        <v>217678</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -11005,7 +11182,7 @@
       </c>
       <c r="E27" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>137908</v>
+        <v>63197</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -11023,7 +11200,7 @@
       </c>
       <c r="E28" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>149458</v>
+        <v>184917</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -11041,7 +11218,7 @@
       </c>
       <c r="E29" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>220158</v>
+        <v>35160</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -11059,7 +11236,7 @@
       </c>
       <c r="E30" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>37364</v>
+        <v>56974</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -11077,7 +11254,7 @@
       </c>
       <c r="E31" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>162370</v>
+        <v>186779</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -11095,7 +11272,7 @@
       </c>
       <c r="E32" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>67152</v>
+        <v>243797</v>
       </c>
     </row>
     <row r="33" spans="1:5">

</xml_diff>

<commit_message>
Add PPL data and targets
One more row of data!
</commit_message>
<xml_diff>
--- a/examples/data/20220215 ITR Tool Sample Data.xlsx
+++ b/examples/data/20220215 ITR Tool Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CF4989-38DB-9044-B4FB-524B19360EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD664DD-4459-BB4D-A540-782F0675653C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44760" yWindow="6520" windowWidth="44560" windowHeight="22440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51600" yWindow="7880" windowWidth="44560" windowHeight="22440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -591,7 +591,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="325">
   <si>
     <t>Data field</t>
   </si>
@@ -3878,11 +3878,11 @@
   </sheetPr>
   <dimension ref="A1:AZ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M32" sqref="M32"/>
+      <selection pane="bottomRight" activeCell="A33" sqref="A33:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -7480,29 +7480,89 @@
       </c>
     </row>
     <row r="33" spans="1:49">
-      <c r="A33" s="61"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="61"/>
-      <c r="L33" s="61"/>
-      <c r="M33" s="61"/>
-      <c r="N33" s="61"/>
-      <c r="O33" s="68"/>
-      <c r="P33" s="68"/>
+      <c r="A33" s="61" t="s">
+        <v>261</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C33" s="61" t="s">
+        <v>263</v>
+      </c>
+      <c r="D33" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H33" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I33" s="5">
+        <v>44196</v>
+      </c>
+      <c r="J33" s="61">
+        <v>19865342074</v>
+      </c>
+      <c r="K33" s="61">
+        <v>7769000000</v>
+      </c>
+      <c r="L33" s="61">
+        <v>40943342074</v>
+      </c>
+      <c r="M33" s="61">
+        <v>41758342074</v>
+      </c>
+      <c r="N33" s="61">
+        <v>45680000000</v>
+      </c>
+      <c r="O33" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P33" s="61" t="s">
+        <v>318</v>
+      </c>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
-      <c r="AS33" s="61"/>
-      <c r="AT33" s="61"/>
-      <c r="AU33" s="61"/>
-      <c r="AV33" s="61"/>
-      <c r="AW33" s="61"/>
+      <c r="AE33" s="69">
+        <v>30.088487220000001</v>
+      </c>
+      <c r="AF33" s="69">
+        <v>30.24837145</v>
+      </c>
+      <c r="AG33" s="69">
+        <v>31.611469039999999</v>
+      </c>
+      <c r="AH33" s="69">
+        <v>28.778915319999999</v>
+      </c>
+      <c r="AI33" s="69">
+        <v>28.07780713</v>
+      </c>
+      <c r="AS33" s="61">
+        <v>38.355258640000002</v>
+      </c>
+      <c r="AT33" s="61">
+        <v>37.442832350000003</v>
+      </c>
+      <c r="AU33" s="61">
+        <v>39.590075179999999</v>
+      </c>
+      <c r="AV33" s="61">
+        <v>35.152931719999998</v>
+      </c>
+      <c r="AW33" s="61">
+        <v>32.487984334642732</v>
+      </c>
     </row>
     <row r="34" spans="1:49">
       <c r="A34" s="61"/>
@@ -7939,10 +7999,10 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9442,10 +9502,82 @@
       </c>
     </row>
     <row r="42" spans="1:12">
-      <c r="I42" s="76"/>
+      <c r="A42" s="61" t="s">
+        <v>261</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C42" s="61" t="s">
+        <v>263</v>
+      </c>
+      <c r="D42" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E42" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F42" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G42" s="61">
+        <v>2021</v>
+      </c>
+      <c r="H42" s="20">
+        <v>2010</v>
+      </c>
+      <c r="I42" s="76">
+        <f>60736086+1597157</f>
+        <v>62333243</v>
+      </c>
+      <c r="J42" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="K42" s="61">
+        <v>2035</v>
+      </c>
+      <c r="L42" s="75">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="43" spans="1:12">
-      <c r="I43" s="76"/>
+      <c r="A43" s="61" t="s">
+        <v>261</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C43" s="61" t="s">
+        <v>263</v>
+      </c>
+      <c r="D43" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F43" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G43" s="61">
+        <v>2021</v>
+      </c>
+      <c r="H43" s="20">
+        <v>2010</v>
+      </c>
+      <c r="I43" s="76">
+        <f>60736086+1597157</f>
+        <v>62333243</v>
+      </c>
+      <c r="J43" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="K43" s="61">
+        <v>2040</v>
+      </c>
+      <c r="L43" s="75">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="44" spans="1:12">
       <c r="I44" s="76"/>
@@ -10688,8 +10820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F8BFE4-8461-B541-8467-258963D3527B}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10732,7 +10864,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>112482</v>
+        <v>72202</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -10750,7 +10882,7 @@
       </c>
       <c r="E3" s="61">
         <f t="shared" ref="E3:E41" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
-        <v>79808</v>
+        <v>73526</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -10768,7 +10900,7 @@
       </c>
       <c r="E4" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>197683</v>
+        <v>240322</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -10786,7 +10918,7 @@
       </c>
       <c r="E5" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>103668</v>
+        <v>107919</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -10804,7 +10936,7 @@
       </c>
       <c r="E6" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>238242</v>
+        <v>72844</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -10822,7 +10954,7 @@
       </c>
       <c r="E7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>44179</v>
+        <v>92782</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -10840,7 +10972,7 @@
       </c>
       <c r="E8" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>61886</v>
+        <v>92119</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10858,7 +10990,7 @@
       </c>
       <c r="E9" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>115388</v>
+        <v>218353</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -10876,7 +11008,7 @@
       </c>
       <c r="E10" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>166584</v>
+        <v>65475</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -10894,7 +11026,7 @@
       </c>
       <c r="E11" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>128579</v>
+        <v>223699</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -10912,7 +11044,7 @@
       </c>
       <c r="E12" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>107445</v>
+        <v>196417</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -10930,7 +11062,7 @@
       </c>
       <c r="E13" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>51498</v>
+        <v>140770</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -10948,7 +11080,7 @@
       </c>
       <c r="E14" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>174097</v>
+        <v>121912</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -10966,7 +11098,7 @@
       </c>
       <c r="E15" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>244975</v>
+        <v>196880</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -10984,7 +11116,7 @@
       </c>
       <c r="E16" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>63648</v>
+        <v>200429</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -11002,7 +11134,7 @@
       </c>
       <c r="E17" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>130212</v>
+        <v>176914</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -11020,7 +11152,7 @@
       </c>
       <c r="E18" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>140402</v>
+        <v>95469</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -11038,7 +11170,7 @@
       </c>
       <c r="E19" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>102138</v>
+        <v>149405</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -11056,7 +11188,7 @@
       </c>
       <c r="E20" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>167696</v>
+        <v>175462</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -11074,7 +11206,7 @@
       </c>
       <c r="E21" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>167039</v>
+        <v>218599</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -11092,7 +11224,7 @@
       </c>
       <c r="E22" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>67866</v>
+        <v>159201</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -11110,7 +11242,7 @@
       </c>
       <c r="E23" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>229436</v>
+        <v>158753</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -11128,7 +11260,7 @@
       </c>
       <c r="E24" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>239933</v>
+        <v>194641</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -11146,7 +11278,7 @@
       </c>
       <c r="E25" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>148946</v>
+        <v>40914</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -11164,7 +11296,7 @@
       </c>
       <c r="E26" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>217678</v>
+        <v>171655</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -11182,7 +11314,7 @@
       </c>
       <c r="E27" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>63197</v>
+        <v>211491</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -11200,7 +11332,7 @@
       </c>
       <c r="E28" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>184917</v>
+        <v>163760</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -11218,7 +11350,7 @@
       </c>
       <c r="E29" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>35160</v>
+        <v>79169</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -11236,7 +11368,7 @@
       </c>
       <c r="E30" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>56974</v>
+        <v>38383</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -11254,7 +11386,7 @@
       </c>
       <c r="E31" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>186779</v>
+        <v>60079</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -11272,15 +11404,26 @@
       </c>
       <c r="E32" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>243797</v>
+        <v>189840</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="68"/>
-      <c r="B33" s="88"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="61"/>
+      <c r="A33" s="61" t="s">
+        <v>261</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C33" s="61" t="s">
+        <v>263</v>
+      </c>
+      <c r="D33" s="61" t="s">
+        <v>263</v>
+      </c>
+      <c r="E33" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>68380</v>
+      </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="68"/>
@@ -11351,10 +11494,10 @@
   <dimension ref="A1:AZ54"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AI22" sqref="AI22"/>
+      <selection pane="bottomRight" activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -15974,7 +16117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B625E0-7A95-AB40-9EC5-2C6C2025FC51}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update template sample data file for Notebook
Some additional data updates were needed to get the template notebook working again.  It is working again now.
</commit_message>
<xml_diff>
--- a/examples/data/20220215 ITR Tool Sample Data.xlsx
+++ b/examples/data/20220215 ITR Tool Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD664DD-4459-BB4D-A540-782F0675653C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC2D88E-09D2-7C45-AFBE-48F94FC59B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51600" yWindow="7880" windowWidth="44560" windowHeight="22440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44680" yWindow="14200" windowWidth="44560" windowHeight="22440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -524,19 +524,8 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>Really S1+S2+S3 but setting to S1+S2 for now.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Really S1+S2+S3 but setting to S1+S2 for now.
 </t>
         </r>
       </text>
@@ -569,19 +558,8 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>Really S1+S2+S3 but setting to S1+S2 for now.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Really S1+S2+S3 but setting to S1+S2 for now.
 </t>
         </r>
       </text>
@@ -591,7 +569,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="324">
   <si>
     <t>Data field</t>
   </si>
@@ -1686,9 +1664,6 @@
   </si>
   <si>
     <t>investment_value</t>
-  </si>
-  <si>
-    <t>Asia</t>
   </si>
   <si>
     <t>netzero_year</t>
@@ -3801,7 +3776,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>123</v>
@@ -3878,11 +3853,11 @@
   </sheetPr>
   <dimension ref="A1:AZ50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A33" sqref="A33:C33"/>
+      <selection pane="bottomRight" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -4073,9 +4048,7 @@
       <c r="D2" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E2" s="61"/>
       <c r="F2" s="61" t="s">
         <v>142</v>
       </c>
@@ -4225,9 +4198,7 @@
       <c r="D3" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E3" s="61"/>
       <c r="F3" s="61" t="s">
         <v>142</v>
       </c>
@@ -4311,9 +4282,7 @@
       <c r="D4" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E4" s="61"/>
       <c r="F4" s="61" t="s">
         <v>142</v>
       </c>
@@ -4430,9 +4399,7 @@
       <c r="D5" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E5" s="61"/>
       <c r="F5" s="61" t="s">
         <v>142</v>
       </c>
@@ -4515,9 +4482,7 @@
       <c r="D6" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E6" s="61"/>
       <c r="F6" s="61" t="s">
         <v>142</v>
       </c>
@@ -4638,9 +4603,7 @@
       <c r="D7" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E7" s="61"/>
       <c r="F7" s="61" t="s">
         <v>142</v>
       </c>
@@ -4770,9 +4733,7 @@
       <c r="D8" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E8" s="61"/>
       <c r="F8" s="61" t="s">
         <v>142</v>
       </c>
@@ -4879,9 +4840,7 @@
       <c r="D9" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E9" s="61"/>
       <c r="F9" s="61" t="s">
         <v>182</v>
       </c>
@@ -4964,9 +4923,7 @@
       <c r="D10" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E10" s="61"/>
       <c r="F10" s="61" t="s">
         <v>142</v>
       </c>
@@ -5050,9 +5007,7 @@
       <c r="D11" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E11" s="61"/>
       <c r="F11" s="61" t="s">
         <v>182</v>
       </c>
@@ -5170,9 +5125,7 @@
       <c r="D12" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E12" s="61"/>
       <c r="F12" s="61" t="s">
         <v>142</v>
       </c>
@@ -5201,7 +5154,7 @@
         <v>7476298000</v>
       </c>
       <c r="O12" s="61" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="P12" s="61" t="s">
         <v>318</v>
@@ -5256,9 +5209,7 @@
       <c r="D13" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E13" s="61"/>
       <c r="F13" s="61" t="s">
         <v>142</v>
       </c>
@@ -5306,6 +5257,49 @@
       </c>
       <c r="U13" s="2">
         <v>1.145419433</v>
+      </c>
+      <c r="X13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="69">
+        <f>IF(OR(ISBLANK(Q13), ISBLANK(X13)),"",Q13+X13)</f>
+        <v>1.325786621</v>
+      </c>
+      <c r="AF13" s="69">
+        <f t="shared" ref="AF13" si="14">IF(ISBLANK(R13),IF(ISBLANK(Y13),"",Y13),R13+Y13)</f>
+        <v>1.323738978</v>
+      </c>
+      <c r="AG13" s="69">
+        <f t="shared" ref="AG13" si="15">IF(ISBLANK(S13),IF(ISBLANK(Z13),"",Z13),S13+Z13)</f>
+        <v>1.2685339369999999</v>
+      </c>
+      <c r="AH13" s="69">
+        <f t="shared" ref="AH13" si="16">IF(ISBLANK(T13),IF(ISBLANK(AA13),"",AA13),T13+AA13)</f>
+        <v>1.202690405</v>
+      </c>
+      <c r="AI13" s="69">
+        <f t="shared" ref="AI13" si="17">IF(ISBLANK(U13),IF(ISBLANK(AB13),"",AB13),U13+AB13)</f>
+        <v>1.145419433</v>
+      </c>
+      <c r="AJ13" s="69" t="str">
+        <f t="shared" ref="AJ13" si="18">IF(ISBLANK(V13),IF(ISBLANK(AC13),"",AC13),V13+AC13)</f>
+        <v/>
+      </c>
+      <c r="AK13" s="69" t="str">
+        <f t="shared" ref="AK13" si="19">IF(ISBLANK(W13),IF(ISBLANK(AD13),"",AD13),W13+AD13)</f>
+        <v/>
       </c>
       <c r="AS13" s="61">
         <v>5.3109194439999996</v>
@@ -5337,9 +5331,7 @@
       <c r="D14" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E14" s="61"/>
       <c r="F14" s="61" t="s">
         <v>142</v>
       </c>
@@ -5387,6 +5379,49 @@
       </c>
       <c r="U14" s="2">
         <v>26.48364437</v>
+      </c>
+      <c r="X14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="69">
+        <f>IF(OR(ISBLANK(Q14), ISBLANK(X14)),"",Q14+X14)</f>
+        <v>26.796145450000001</v>
+      </c>
+      <c r="AF14" s="69">
+        <f t="shared" ref="AF14" si="20">IF(ISBLANK(R14),IF(ISBLANK(Y14),"",Y14),R14+Y14)</f>
+        <v>27.947696990000001</v>
+      </c>
+      <c r="AG14" s="69">
+        <f t="shared" ref="AG14" si="21">IF(ISBLANK(S14),IF(ISBLANK(Z14),"",Z14),S14+Z14)</f>
+        <v>29.95633261</v>
+      </c>
+      <c r="AH14" s="69">
+        <f t="shared" ref="AH14" si="22">IF(ISBLANK(T14),IF(ISBLANK(AA14),"",AA14),T14+AA14)</f>
+        <v>27.00027425</v>
+      </c>
+      <c r="AI14" s="69">
+        <f t="shared" ref="AI14" si="23">IF(ISBLANK(U14),IF(ISBLANK(AB14),"",AB14),U14+AB14)</f>
+        <v>26.48364437</v>
+      </c>
+      <c r="AJ14" s="69" t="str">
+        <f t="shared" ref="AJ14" si="24">IF(ISBLANK(V14),IF(ISBLANK(AC14),"",AC14),V14+AC14)</f>
+        <v/>
+      </c>
+      <c r="AK14" s="69" t="str">
+        <f t="shared" ref="AK14" si="25">IF(ISBLANK(W14),IF(ISBLANK(AD14),"",AD14),W14+AD14)</f>
+        <v/>
       </c>
       <c r="AS14" s="61">
         <v>39.339109710000002</v>
@@ -5418,9 +5453,7 @@
       <c r="D15" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E15" s="61"/>
       <c r="F15" s="61" t="s">
         <v>142</v>
       </c>
@@ -5518,9 +5551,7 @@
       <c r="D16" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E16" s="61"/>
       <c r="F16" s="61" t="s">
         <v>142</v>
       </c>
@@ -5568,6 +5599,49 @@
       </c>
       <c r="U16" s="2">
         <v>82.018839239000002</v>
+      </c>
+      <c r="X16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="69">
+        <f t="shared" ref="AE16:AE17" si="26">IF(OR(ISBLANK(Q16), ISBLANK(X16)),"",Q16+X16)</f>
+        <v>94.923459879999996</v>
+      </c>
+      <c r="AF16" s="69">
+        <f t="shared" ref="AF16:AF17" si="27">IF(ISBLANK(R16),IF(ISBLANK(Y16),"",Y16),R16+Y16)</f>
+        <v>93.530450478000006</v>
+      </c>
+      <c r="AG16" s="69">
+        <f t="shared" ref="AG16:AG17" si="28">IF(ISBLANK(S16),IF(ISBLANK(Z16),"",Z16),S16+Z16)</f>
+        <v>95.012237693000003</v>
+      </c>
+      <c r="AH16" s="69">
+        <f t="shared" ref="AH16:AH17" si="29">IF(ISBLANK(T16),IF(ISBLANK(AA16),"",AA16),T16+AA16)</f>
+        <v>83.595723118999999</v>
+      </c>
+      <c r="AI16" s="69">
+        <f t="shared" ref="AI16:AI17" si="30">IF(ISBLANK(U16),IF(ISBLANK(AB16),"",AB16),U16+AB16)</f>
+        <v>82.018839239000002</v>
+      </c>
+      <c r="AJ16" s="69" t="str">
+        <f t="shared" ref="AJ16:AJ17" si="31">IF(ISBLANK(V16),IF(ISBLANK(AC16),"",AC16),V16+AC16)</f>
+        <v/>
+      </c>
+      <c r="AK16" s="69" t="str">
+        <f t="shared" ref="AK16:AK17" si="32">IF(ISBLANK(W16),IF(ISBLANK(AD16),"",AD16),W16+AD16)</f>
+        <v/>
       </c>
       <c r="AS16" s="61">
         <v>221.77898501999999</v>
@@ -5599,9 +5673,7 @@
       <c r="D17" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E17" s="61"/>
       <c r="F17" s="61" t="s">
         <v>142</v>
       </c>
@@ -5649,6 +5721,49 @@
       </c>
       <c r="U17" s="90">
         <v>33.246229124999999</v>
+      </c>
+      <c r="X17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="69">
+        <f t="shared" si="26"/>
+        <v>32.516193991999998</v>
+      </c>
+      <c r="AF17" s="69">
+        <f t="shared" si="27"/>
+        <v>31.450986952000001</v>
+      </c>
+      <c r="AG17" s="69">
+        <f t="shared" si="28"/>
+        <v>34.631975513</v>
+      </c>
+      <c r="AH17" s="69">
+        <f t="shared" si="29"/>
+        <v>33.246229124999999</v>
+      </c>
+      <c r="AI17" s="69">
+        <f t="shared" si="30"/>
+        <v>33.246229124999999</v>
+      </c>
+      <c r="AJ17" s="69" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="AK17" s="69" t="str">
+        <f t="shared" si="32"/>
+        <v/>
       </c>
       <c r="AS17" s="61">
         <v>102.999524264</v>
@@ -5680,9 +5795,7 @@
       <c r="D18" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E18" s="61"/>
       <c r="F18" s="61" t="s">
         <v>142</v>
       </c>
@@ -5747,31 +5860,31 @@
         <v>0</v>
       </c>
       <c r="AE18" s="69">
-        <f t="shared" ref="AE18" si="14">IF(OR(ISBLANK(Q18), ISBLANK(X18)),"",Q18+X18)</f>
+        <f t="shared" ref="AE18" si="33">IF(OR(ISBLANK(Q18), ISBLANK(X18)),"",Q18+X18)</f>
         <v>35.122915438000007</v>
       </c>
       <c r="AF18" s="69">
-        <f t="shared" ref="AF18" si="15">IF(OR(ISBLANK(R18), ISBLANK(Y18)),"",R18+Y18)</f>
+        <f t="shared" ref="AF18" si="34">IF(OR(ISBLANK(R18), ISBLANK(Y18)),"",R18+Y18)</f>
         <v>32.270565695999998</v>
       </c>
       <c r="AG18" s="69">
-        <f t="shared" ref="AG18" si="16">IF(OR(ISBLANK(S18), ISBLANK(Z18)),"",S18+Z18)</f>
+        <f t="shared" ref="AG18" si="35">IF(OR(ISBLANK(S18), ISBLANK(Z18)),"",S18+Z18)</f>
         <v>28.483757178000001</v>
       </c>
       <c r="AH18" s="69">
-        <f t="shared" ref="AH18" si="17">IF(OR(ISBLANK(T18), ISBLANK(AA18)),"",T18+AA18)</f>
+        <f t="shared" ref="AH18" si="36">IF(OR(ISBLANK(T18), ISBLANK(AA18)),"",T18+AA18)</f>
         <v>26.74941115</v>
       </c>
       <c r="AI18" s="69">
-        <f t="shared" ref="AI18" si="18">IF(OR(ISBLANK(U18), ISBLANK(AB18)),"",U18+AB18)</f>
+        <f t="shared" ref="AI18" si="37">IF(OR(ISBLANK(U18), ISBLANK(AB18)),"",U18+AB18)</f>
         <v>35.013482494000002</v>
       </c>
       <c r="AJ18" s="69" t="str">
-        <f t="shared" ref="AJ18" si="19">IF(OR(ISBLANK(V18), ISBLANK(AC18)),"",V18+AC18)</f>
+        <f t="shared" ref="AJ18" si="38">IF(OR(ISBLANK(V18), ISBLANK(AC18)),"",V18+AC18)</f>
         <v/>
       </c>
       <c r="AK18" s="69" t="str">
-        <f t="shared" ref="AK18" si="20">IF(OR(ISBLANK(W18), ISBLANK(AD18)),"",W18+AD18)</f>
+        <f t="shared" ref="AK18" si="39">IF(OR(ISBLANK(W18), ISBLANK(AD18)),"",W18+AD18)</f>
         <v/>
       </c>
       <c r="AS18" s="61">
@@ -5804,9 +5917,7 @@
       <c r="D19" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E19" s="61"/>
       <c r="F19" s="61" t="s">
         <v>142</v>
       </c>
@@ -5872,31 +5983,31 @@
         <v>0</v>
       </c>
       <c r="AE19" s="69">
-        <f t="shared" ref="AE19" si="21">IF(OR(ISBLANK(Q19), ISBLANK(X19)),"",Q19+X19)</f>
+        <f t="shared" ref="AE19" si="40">IF(OR(ISBLANK(Q19), ISBLANK(X19)),"",Q19+X19)</f>
         <v>0.54127069000000005</v>
       </c>
       <c r="AF19" s="69">
-        <f t="shared" ref="AF19" si="22">IF(OR(ISBLANK(R19), ISBLANK(Y19)),"",R19+Y19)</f>
+        <f t="shared" ref="AF19" si="41">IF(OR(ISBLANK(R19), ISBLANK(Y19)),"",R19+Y19)</f>
         <v>0.38852905199999999</v>
       </c>
       <c r="AG19" s="69">
-        <f t="shared" ref="AG19" si="23">IF(OR(ISBLANK(S19), ISBLANK(Z19)),"",S19+Z19)</f>
+        <f t="shared" ref="AG19" si="42">IF(OR(ISBLANK(S19), ISBLANK(Z19)),"",S19+Z19)</f>
         <v>3.4941450000000002E-3</v>
       </c>
       <c r="AH19" s="69">
-        <f t="shared" ref="AH19" si="24">IF(OR(ISBLANK(T19), ISBLANK(AA19)),"",T19+AA19)</f>
+        <f t="shared" ref="AH19" si="43">IF(OR(ISBLANK(T19), ISBLANK(AA19)),"",T19+AA19)</f>
         <v>2.2128600000000001E-4</v>
       </c>
       <c r="AI19" s="69">
-        <f t="shared" ref="AI19" si="25">IF(OR(ISBLANK(U19), ISBLANK(AB19)),"",U19+AB19)</f>
+        <f t="shared" ref="AI19" si="44">IF(OR(ISBLANK(U19), ISBLANK(AB19)),"",U19+AB19)</f>
         <v>2.2128600000000001E-4</v>
       </c>
       <c r="AJ19" s="69" t="str">
-        <f t="shared" ref="AJ19" si="26">IF(OR(ISBLANK(V19), ISBLANK(AC19)),"",V19+AC19)</f>
+        <f t="shared" ref="AJ19" si="45">IF(OR(ISBLANK(V19), ISBLANK(AC19)),"",V19+AC19)</f>
         <v/>
       </c>
       <c r="AK19" s="69" t="str">
-        <f t="shared" ref="AK19" si="27">IF(OR(ISBLANK(W19), ISBLANK(AD19)),"",W19+AD19)</f>
+        <f t="shared" ref="AK19" si="46">IF(OR(ISBLANK(W19), ISBLANK(AD19)),"",W19+AD19)</f>
         <v/>
       </c>
       <c r="AS19" s="61">
@@ -5928,9 +6039,7 @@
       <c r="D20" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E20" s="61"/>
       <c r="F20" s="61" t="s">
         <v>142</v>
       </c>
@@ -5999,27 +6108,27 @@
         <v>16784000</v>
       </c>
       <c r="AF20" s="69">
-        <f t="shared" ref="AF20" si="28">IF(ISBLANK(R20),IF(ISBLANK(Y20),"",Y20),R20+Y20)</f>
+        <f t="shared" ref="AF20" si="47">IF(ISBLANK(R20),IF(ISBLANK(Y20),"",Y20),R20+Y20)</f>
         <v>27225000</v>
       </c>
       <c r="AG20" s="69">
-        <f t="shared" ref="AG20" si="29">IF(ISBLANK(S20),IF(ISBLANK(Z20),"",Z20),S20+Z20)</f>
+        <f t="shared" ref="AG20" si="48">IF(ISBLANK(S20),IF(ISBLANK(Z20),"",Z20),S20+Z20)</f>
         <v>29863000</v>
       </c>
       <c r="AH20" s="69">
-        <f t="shared" ref="AH20" si="30">IF(ISBLANK(T20),IF(ISBLANK(AA20),"",AA20),T20+AA20)</f>
+        <f t="shared" ref="AH20" si="49">IF(ISBLANK(T20),IF(ISBLANK(AA20),"",AA20),T20+AA20)</f>
         <v>27430000</v>
       </c>
       <c r="AI20" s="69">
-        <f t="shared" ref="AI20" si="31">IF(ISBLANK(U20),IF(ISBLANK(AB20),"",AB20),U20+AB20)</f>
+        <f t="shared" ref="AI20" si="50">IF(ISBLANK(U20),IF(ISBLANK(AB20),"",AB20),U20+AB20)</f>
         <v>22213000</v>
       </c>
       <c r="AJ20" s="69" t="str">
-        <f t="shared" ref="AJ20" si="32">IF(ISBLANK(V20),IF(ISBLANK(AC20),"",AC20),V20+AC20)</f>
+        <f t="shared" ref="AJ20" si="51">IF(ISBLANK(V20),IF(ISBLANK(AC20),"",AC20),V20+AC20)</f>
         <v/>
       </c>
       <c r="AK20" s="69" t="str">
-        <f t="shared" ref="AK20" si="33">IF(ISBLANK(W20),IF(ISBLANK(AD20),"",AD20),W20+AD20)</f>
+        <f t="shared" ref="AK20" si="52">IF(ISBLANK(W20),IF(ISBLANK(AD20),"",AD20),W20+AD20)</f>
         <v/>
       </c>
       <c r="AS20" s="76">
@@ -6054,9 +6163,7 @@
       <c r="D21" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E21" s="61"/>
       <c r="F21" s="61" t="s">
         <v>142</v>
       </c>
@@ -6120,27 +6227,27 @@
         <v/>
       </c>
       <c r="AF21" s="69">
-        <f t="shared" ref="AF21" si="34">IF(ISBLANK(R21),IF(ISBLANK(Y21),"",Y21),R21+Y21)</f>
+        <f t="shared" ref="AF21" si="53">IF(ISBLANK(R21),IF(ISBLANK(Y21),"",Y21),R21+Y21)</f>
         <v>60434671</v>
       </c>
       <c r="AG21" s="69">
-        <f t="shared" ref="AG21" si="35">IF(ISBLANK(S21),IF(ISBLANK(Z21),"",Z21),S21+Z21)</f>
+        <f t="shared" ref="AG21" si="54">IF(ISBLANK(S21),IF(ISBLANK(Z21),"",Z21),S21+Z21)</f>
         <v>52972697</v>
       </c>
       <c r="AH21" s="69">
-        <f t="shared" ref="AH21" si="36">IF(ISBLANK(T21),IF(ISBLANK(AA21),"",AA21),T21+AA21)</f>
+        <f t="shared" ref="AH21" si="55">IF(ISBLANK(T21),IF(ISBLANK(AA21),"",AA21),T21+AA21)</f>
         <v>49863111</v>
       </c>
       <c r="AI21" s="69">
-        <f t="shared" ref="AI21" si="37">IF(ISBLANK(U21),IF(ISBLANK(AB21),"",AB21),U21+AB21)</f>
+        <f t="shared" ref="AI21" si="56">IF(ISBLANK(U21),IF(ISBLANK(AB21),"",AB21),U21+AB21)</f>
         <v>42750225</v>
       </c>
       <c r="AJ21" s="69" t="str">
-        <f t="shared" ref="AJ21" si="38">IF(ISBLANK(V21),IF(ISBLANK(AC21),"",AC21),V21+AC21)</f>
+        <f t="shared" ref="AJ21" si="57">IF(ISBLANK(V21),IF(ISBLANK(AC21),"",AC21),V21+AC21)</f>
         <v/>
       </c>
       <c r="AK21" s="69" t="str">
-        <f t="shared" ref="AK21" si="39">IF(ISBLANK(W21),IF(ISBLANK(AD21),"",AD21),W21+AD21)</f>
+        <f t="shared" ref="AK21" si="58">IF(ISBLANK(W21),IF(ISBLANK(AD21),"",AD21),W21+AD21)</f>
         <v/>
       </c>
       <c r="AS21" s="61"/>
@@ -6170,9 +6277,7 @@
       <c r="D22" s="61" t="s">
         <v>154</v>
       </c>
-      <c r="E22" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E22" s="61"/>
       <c r="F22" s="61" t="s">
         <v>142</v>
       </c>
@@ -6241,31 +6346,31 @@
         <v>2487000</v>
       </c>
       <c r="AE22" s="69">
-        <f t="shared" ref="AE22:AK23" si="40">IF(OR(ISBLANK(Q22), ISBLANK(X22)),"",Q22+X22)</f>
+        <f t="shared" ref="AE22:AK23" si="59">IF(OR(ISBLANK(Q22), ISBLANK(X22)),"",Q22+X22)</f>
         <v>14435000</v>
       </c>
       <c r="AF22" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>13858000</v>
       </c>
       <c r="AG22" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>13933000</v>
       </c>
       <c r="AH22" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>14858000</v>
       </c>
       <c r="AI22" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>12580000</v>
       </c>
       <c r="AJ22" s="69" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v/>
       </c>
       <c r="AK22" s="69" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v/>
       </c>
       <c r="AS22" s="61">
@@ -6302,9 +6407,7 @@
       <c r="D23" s="61" t="s">
         <v>226</v>
       </c>
-      <c r="E23" s="61" t="s">
-        <v>227</v>
-      </c>
+      <c r="E23" s="61"/>
       <c r="F23" s="61" t="s">
         <v>182</v>
       </c>
@@ -6370,31 +6473,31 @@
         <v>0</v>
       </c>
       <c r="AE23" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>16.100000000000001</v>
       </c>
       <c r="AF23" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>16.100000000000001</v>
       </c>
       <c r="AG23" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>14.27265885416667</v>
       </c>
       <c r="AH23" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>11.947505</v>
       </c>
       <c r="AI23" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>11.738147617323991</v>
       </c>
       <c r="AJ23" s="69" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v/>
       </c>
       <c r="AK23" s="69" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v/>
       </c>
       <c r="AS23" s="61">
@@ -6426,9 +6529,7 @@
       <c r="D24" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E24" s="61"/>
       <c r="F24" s="61" t="s">
         <v>142</v>
       </c>
@@ -6493,31 +6594,31 @@
         <v>0</v>
       </c>
       <c r="AE24" s="69">
-        <f t="shared" ref="AE24" si="41">IF(OR(ISBLANK(Q24), ISBLANK(X24)),"",Q24+X24)</f>
+        <f t="shared" ref="AE24" si="60">IF(OR(ISBLANK(Q24), ISBLANK(X24)),"",Q24+X24)</f>
         <v>3.8868941879999999</v>
       </c>
       <c r="AF24" s="69">
-        <f t="shared" ref="AF24" si="42">IF(OR(ISBLANK(R24), ISBLANK(Y24)),"",R24+Y24)</f>
+        <f t="shared" ref="AF24" si="61">IF(OR(ISBLANK(R24), ISBLANK(Y24)),"",R24+Y24)</f>
         <v>3.8663196809999998</v>
       </c>
       <c r="AG24" s="69">
-        <f t="shared" ref="AG24" si="43">IF(OR(ISBLANK(S24), ISBLANK(Z24)),"",S24+Z24)</f>
+        <f t="shared" ref="AG24" si="62">IF(OR(ISBLANK(S24), ISBLANK(Z24)),"",S24+Z24)</f>
         <v>3.937301664</v>
       </c>
       <c r="AH24" s="69">
-        <f t="shared" ref="AH24" si="44">IF(OR(ISBLANK(T24), ISBLANK(AA24)),"",T24+AA24)</f>
+        <f t="shared" ref="AH24" si="63">IF(OR(ISBLANK(T24), ISBLANK(AA24)),"",T24+AA24)</f>
         <v>3.9790181429999998</v>
       </c>
       <c r="AI24" s="69">
-        <f t="shared" ref="AI24" si="45">IF(OR(ISBLANK(U24), ISBLANK(AB24)),"",U24+AB24)</f>
+        <f t="shared" ref="AI24" si="64">IF(OR(ISBLANK(U24), ISBLANK(AB24)),"",U24+AB24)</f>
         <v>3.8259789839999998</v>
       </c>
       <c r="AJ24" s="69" t="str">
-        <f t="shared" ref="AJ24" si="46">IF(OR(ISBLANK(V24), ISBLANK(AC24)),"",V24+AC24)</f>
+        <f t="shared" ref="AJ24" si="65">IF(OR(ISBLANK(V24), ISBLANK(AC24)),"",V24+AC24)</f>
         <v/>
       </c>
       <c r="AK24" s="69" t="str">
-        <f t="shared" ref="AK24" si="47">IF(OR(ISBLANK(W24), ISBLANK(AD24)),"",W24+AD24)</f>
+        <f t="shared" ref="AK24" si="66">IF(OR(ISBLANK(W24), ISBLANK(AD24)),"",W24+AD24)</f>
         <v/>
       </c>
       <c r="AS24" s="61">
@@ -6549,9 +6650,7 @@
       <c r="D25" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E25" s="61"/>
       <c r="F25" s="61" t="s">
         <v>142</v>
       </c>
@@ -6617,31 +6716,31 @@
         <v>0</v>
       </c>
       <c r="AE25" s="69">
-        <f t="shared" ref="AE25:AE27" si="48">IF(OR(ISBLANK(Q25), ISBLANK(X25)),"",Q25+X25)</f>
+        <f t="shared" ref="AE25:AE27" si="67">IF(OR(ISBLANK(Q25), ISBLANK(X25)),"",Q25+X25)</f>
         <v>1.8746218750000001</v>
       </c>
       <c r="AF25" s="69">
-        <f t="shared" ref="AF25:AF27" si="49">IF(OR(ISBLANK(R25), ISBLANK(Y25)),"",R25+Y25)</f>
+        <f t="shared" ref="AF25:AF27" si="68">IF(OR(ISBLANK(R25), ISBLANK(Y25)),"",R25+Y25)</f>
         <v>1.844359927</v>
       </c>
       <c r="AG25" s="69">
-        <f t="shared" ref="AG25:AG27" si="50">IF(OR(ISBLANK(S25), ISBLANK(Z25)),"",S25+Z25)</f>
+        <f t="shared" ref="AG25:AG27" si="69">IF(OR(ISBLANK(S25), ISBLANK(Z25)),"",S25+Z25)</f>
         <v>2.051568649</v>
       </c>
       <c r="AH25" s="69">
-        <f t="shared" ref="AH25:AH27" si="51">IF(OR(ISBLANK(T25), ISBLANK(AA25)),"",T25+AA25)</f>
+        <f t="shared" ref="AH25:AH27" si="70">IF(OR(ISBLANK(T25), ISBLANK(AA25)),"",T25+AA25)</f>
         <v>1.710493431</v>
       </c>
       <c r="AI25" s="69">
-        <f t="shared" ref="AI25:AI27" si="52">IF(OR(ISBLANK(U25), ISBLANK(AB25)),"",U25+AB25)</f>
+        <f t="shared" ref="AI25:AI27" si="71">IF(OR(ISBLANK(U25), ISBLANK(AB25)),"",U25+AB25)</f>
         <v>1.6449851719404254</v>
       </c>
       <c r="AJ25" s="69" t="str">
-        <f t="shared" ref="AJ25:AJ27" si="53">IF(OR(ISBLANK(V25), ISBLANK(AC25)),"",V25+AC25)</f>
+        <f t="shared" ref="AJ25:AJ27" si="72">IF(OR(ISBLANK(V25), ISBLANK(AC25)),"",V25+AC25)</f>
         <v/>
       </c>
       <c r="AK25" s="69" t="str">
-        <f t="shared" ref="AK25:AK27" si="54">IF(OR(ISBLANK(W25), ISBLANK(AD25)),"",W25+AD25)</f>
+        <f t="shared" ref="AK25:AK27" si="73">IF(OR(ISBLANK(W25), ISBLANK(AD25)),"",W25+AD25)</f>
         <v/>
       </c>
       <c r="AS25" s="61">
@@ -6673,9 +6772,7 @@
       <c r="D26" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E26" s="61"/>
       <c r="F26" s="61" t="s">
         <v>182</v>
       </c>
@@ -6740,31 +6837,31 @@
         <v>0</v>
       </c>
       <c r="AE26" s="69">
-        <f t="shared" si="48"/>
+        <f t="shared" si="67"/>
         <v>12.356382978723399</v>
       </c>
       <c r="AF26" s="69">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>11.819148936170221</v>
       </c>
       <c r="AG26" s="69">
-        <f t="shared" si="50"/>
+        <f t="shared" si="69"/>
         <v>11.281914893617021</v>
       </c>
       <c r="AH26" s="69">
-        <f t="shared" si="51"/>
+        <f t="shared" si="70"/>
         <v>10.1</v>
       </c>
       <c r="AI26" s="69">
-        <f t="shared" si="52"/>
+        <f t="shared" si="71"/>
         <v>10.1</v>
       </c>
       <c r="AJ26" s="69" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="72"/>
         <v/>
       </c>
       <c r="AK26" s="69" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="73"/>
         <v/>
       </c>
       <c r="AS26" s="61">
@@ -6796,9 +6893,7 @@
       <c r="D27" s="61" t="s">
         <v>240</v>
       </c>
-      <c r="E27" s="61" t="s">
-        <v>241</v>
-      </c>
+      <c r="E27" s="61"/>
       <c r="F27" s="61" t="s">
         <v>142</v>
       </c>
@@ -6863,31 +6958,31 @@
         <v>0</v>
       </c>
       <c r="AE27" s="69">
-        <f t="shared" si="48"/>
+        <f t="shared" si="67"/>
         <v>3.004725724</v>
       </c>
       <c r="AF27" s="69">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>2.1325357700000001</v>
       </c>
       <c r="AG27" s="69">
-        <f t="shared" si="50"/>
+        <f t="shared" si="69"/>
         <v>3.0720788620000001</v>
       </c>
       <c r="AH27" s="69">
-        <f t="shared" si="51"/>
+        <f t="shared" si="70"/>
         <v>2.4277569909999999</v>
       </c>
       <c r="AI27" s="69">
-        <f t="shared" si="52"/>
+        <f t="shared" si="71"/>
         <v>1.335266345</v>
       </c>
       <c r="AJ27" s="69" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="72"/>
         <v/>
       </c>
       <c r="AK27" s="69" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="73"/>
         <v/>
       </c>
       <c r="AS27" s="61">
@@ -6919,9 +7014,7 @@
       <c r="D28" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E28" s="61"/>
       <c r="F28" s="61" t="s">
         <v>142</v>
       </c>
@@ -6986,31 +7079,31 @@
         <v>0</v>
       </c>
       <c r="AE28" s="69">
-        <f t="shared" ref="AE28" si="55">IF(OR(ISBLANK(Q28), ISBLANK(X28)),"",Q28+X28)</f>
+        <f t="shared" ref="AE28" si="74">IF(OR(ISBLANK(Q28), ISBLANK(X28)),"",Q28+X28)</f>
         <v>0.99625009600000003</v>
       </c>
       <c r="AF28" s="69">
-        <f t="shared" ref="AF28" si="56">IF(OR(ISBLANK(R28), ISBLANK(Y28)),"",R28+Y28)</f>
+        <f t="shared" ref="AF28" si="75">IF(OR(ISBLANK(R28), ISBLANK(Y28)),"",R28+Y28)</f>
         <v>0.98354598199999999</v>
       </c>
       <c r="AG28" s="69">
-        <f t="shared" ref="AG28" si="57">IF(OR(ISBLANK(S28), ISBLANK(Z28)),"",S28+Z28)</f>
+        <f t="shared" ref="AG28" si="76">IF(OR(ISBLANK(S28), ISBLANK(Z28)),"",S28+Z28)</f>
         <v>2.6019487300000002</v>
       </c>
       <c r="AH28" s="69">
-        <f t="shared" ref="AH28" si="58">IF(OR(ISBLANK(T28), ISBLANK(AA28)),"",T28+AA28)</f>
+        <f t="shared" ref="AH28" si="77">IF(OR(ISBLANK(T28), ISBLANK(AA28)),"",T28+AA28)</f>
         <v>2.5352979329999998</v>
       </c>
       <c r="AI28" s="69">
-        <f t="shared" ref="AI28" si="59">IF(OR(ISBLANK(U28), ISBLANK(AB28)),"",U28+AB28)</f>
+        <f t="shared" ref="AI28" si="78">IF(OR(ISBLANK(U28), ISBLANK(AB28)),"",U28+AB28)</f>
         <v>1.926808946</v>
       </c>
       <c r="AJ28" s="69" t="str">
-        <f t="shared" ref="AJ28" si="60">IF(OR(ISBLANK(V28), ISBLANK(AC28)),"",V28+AC28)</f>
+        <f t="shared" ref="AJ28" si="79">IF(OR(ISBLANK(V28), ISBLANK(AC28)),"",V28+AC28)</f>
         <v/>
       </c>
       <c r="AK28" s="69" t="str">
-        <f t="shared" ref="AK28" si="61">IF(OR(ISBLANK(W28), ISBLANK(AD28)),"",W28+AD28)</f>
+        <f t="shared" ref="AK28" si="80">IF(OR(ISBLANK(W28), ISBLANK(AD28)),"",W28+AD28)</f>
         <v/>
       </c>
       <c r="AS28" s="61">
@@ -7042,9 +7135,7 @@
       <c r="D29" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E29" s="61"/>
       <c r="F29" s="61" t="s">
         <v>142</v>
       </c>
@@ -7109,31 +7200,31 @@
         <v>6063090</v>
       </c>
       <c r="AE29" s="69">
-        <f t="shared" ref="AE29:AE30" si="62">IF(OR(ISBLANK(Q29), ISBLANK(X29)),"",Q29+X29)</f>
+        <f t="shared" ref="AE29:AE31" si="81">IF(OR(ISBLANK(Q29), ISBLANK(X29)),"",Q29+X29)</f>
         <v>33167324</v>
       </c>
       <c r="AF29" s="69">
-        <f t="shared" ref="AF29:AF30" si="63">IF(OR(ISBLANK(R29), ISBLANK(Y29)),"",R29+Y29)</f>
+        <f t="shared" ref="AF29:AF30" si="82">IF(OR(ISBLANK(R29), ISBLANK(Y29)),"",R29+Y29)</f>
         <v>36362250</v>
       </c>
       <c r="AG29" s="69">
-        <f t="shared" ref="AG29:AG30" si="64">IF(OR(ISBLANK(S29), ISBLANK(Z29)),"",S29+Z29)</f>
+        <f t="shared" ref="AG29:AG30" si="83">IF(OR(ISBLANK(S29), ISBLANK(Z29)),"",S29+Z29)</f>
         <v>35896971</v>
       </c>
       <c r="AH29" s="69">
-        <f t="shared" ref="AH29:AH30" si="65">IF(OR(ISBLANK(T29), ISBLANK(AA29)),"",T29+AA29)</f>
+        <f t="shared" ref="AH29:AH30" si="84">IF(OR(ISBLANK(T29), ISBLANK(AA29)),"",T29+AA29)</f>
         <v>30327168</v>
       </c>
       <c r="AI29" s="69">
-        <f t="shared" ref="AI29:AI30" si="66">IF(OR(ISBLANK(U29), ISBLANK(AB29)),"",U29+AB29)</f>
+        <f t="shared" ref="AI29:AI30" si="85">IF(OR(ISBLANK(U29), ISBLANK(AB29)),"",U29+AB29)</f>
         <v>31822330</v>
       </c>
       <c r="AJ29" s="69" t="str">
-        <f t="shared" ref="AJ29:AJ30" si="67">IF(OR(ISBLANK(V29), ISBLANK(AC29)),"",V29+AC29)</f>
+        <f t="shared" ref="AJ29:AJ30" si="86">IF(OR(ISBLANK(V29), ISBLANK(AC29)),"",V29+AC29)</f>
         <v/>
       </c>
       <c r="AK29" s="69" t="str">
-        <f t="shared" ref="AK29:AK30" si="68">IF(OR(ISBLANK(W29), ISBLANK(AD29)),"",W29+AD29)</f>
+        <f t="shared" ref="AK29:AK30" si="87">IF(OR(ISBLANK(W29), ISBLANK(AD29)),"",W29+AD29)</f>
         <v/>
       </c>
       <c r="AS29" s="1">
@@ -7170,9 +7261,7 @@
       <c r="D30" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E30" s="61"/>
       <c r="F30" s="61" t="s">
         <v>142</v>
       </c>
@@ -7237,31 +7326,31 @@
         <v>0</v>
       </c>
       <c r="AE30" s="69">
-        <f t="shared" si="62"/>
+        <f t="shared" si="81"/>
         <v>2.2165439930000002</v>
       </c>
       <c r="AF30" s="69">
-        <f t="shared" si="63"/>
+        <f t="shared" si="82"/>
         <v>2.2511915660000001</v>
       </c>
       <c r="AG30" s="69">
-        <f t="shared" si="64"/>
+        <f t="shared" si="83"/>
         <v>2.4511497719999999</v>
       </c>
       <c r="AH30" s="69">
-        <f t="shared" si="65"/>
+        <f t="shared" si="84"/>
         <v>2.4417731950000001</v>
       </c>
       <c r="AI30" s="69">
-        <f t="shared" si="66"/>
+        <f t="shared" si="85"/>
         <v>2.3478588409999999</v>
       </c>
       <c r="AJ30" s="69" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="86"/>
         <v/>
       </c>
       <c r="AK30" s="69" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="87"/>
         <v/>
       </c>
       <c r="AS30" s="61">
@@ -7293,9 +7382,7 @@
       <c r="D31" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E31" s="61"/>
       <c r="F31" s="61" t="s">
         <v>142</v>
       </c>
@@ -7343,6 +7430,49 @@
       </c>
       <c r="U31" s="2">
         <v>5.0787910969999999</v>
+      </c>
+      <c r="X31" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="69">
+        <f t="shared" si="81"/>
+        <v>6.3372507860000002</v>
+      </c>
+      <c r="AF31" s="69">
+        <f t="shared" ref="AF31" si="88">IF(ISBLANK(R31),IF(ISBLANK(Y31),"",Y31),R31+Y31)</f>
+        <v>6.1180013459999998</v>
+      </c>
+      <c r="AG31" s="69">
+        <f t="shared" ref="AG31" si="89">IF(ISBLANK(S31),IF(ISBLANK(Z31),"",Z31),S31+Z31)</f>
+        <v>5.2178957580000001</v>
+      </c>
+      <c r="AH31" s="69">
+        <f t="shared" ref="AH31" si="90">IF(ISBLANK(T31),IF(ISBLANK(AA31),"",AA31),T31+AA31)</f>
+        <v>5.3678279890000002</v>
+      </c>
+      <c r="AI31" s="69">
+        <f t="shared" ref="AI31" si="91">IF(ISBLANK(U31),IF(ISBLANK(AB31),"",AB31),U31+AB31)</f>
+        <v>5.0787910969999999</v>
+      </c>
+      <c r="AJ31" s="69" t="str">
+        <f t="shared" ref="AJ31" si="92">IF(ISBLANK(V31),IF(ISBLANK(AC31),"",AC31),V31+AC31)</f>
+        <v/>
+      </c>
+      <c r="AK31" s="69" t="str">
+        <f t="shared" ref="AK31" si="93">IF(ISBLANK(W31),IF(ISBLANK(AD31),"",AD31),W31+AD31)</f>
+        <v/>
       </c>
       <c r="AS31" s="61">
         <v>11.83516337</v>
@@ -7373,9 +7503,7 @@
       <c r="D32" s="61" t="s">
         <v>260</v>
       </c>
-      <c r="E32" s="61" t="s">
-        <v>323</v>
-      </c>
+      <c r="E32" s="61"/>
       <c r="F32" s="61" t="s">
         <v>182</v>
       </c>
@@ -7438,31 +7566,31 @@
         <v>0</v>
       </c>
       <c r="AE32" s="69" t="str">
-        <f t="shared" ref="AE32" si="69">IF(OR(ISBLANK(Q32), ISBLANK(X32)),"",Q32+X32)</f>
+        <f t="shared" ref="AE32" si="94">IF(OR(ISBLANK(Q32), ISBLANK(X32)),"",Q32+X32)</f>
         <v/>
       </c>
       <c r="AF32" s="69">
-        <f t="shared" ref="AF32" si="70">IF(OR(ISBLANK(R32), ISBLANK(Y32)),"",R32+Y32)</f>
+        <f t="shared" ref="AF32" si="95">IF(OR(ISBLANK(R32), ISBLANK(Y32)),"",R32+Y32)</f>
         <v>78.8</v>
       </c>
       <c r="AG32" s="69">
-        <f t="shared" ref="AG32" si="71">IF(OR(ISBLANK(S32), ISBLANK(Z32)),"",S32+Z32)</f>
+        <f t="shared" ref="AG32" si="96">IF(OR(ISBLANK(S32), ISBLANK(Z32)),"",S32+Z32)</f>
         <v>78.8</v>
       </c>
       <c r="AH32" s="69">
-        <f t="shared" ref="AH32" si="72">IF(OR(ISBLANK(T32), ISBLANK(AA32)),"",T32+AA32)</f>
+        <f t="shared" ref="AH32" si="97">IF(OR(ISBLANK(T32), ISBLANK(AA32)),"",T32+AA32)</f>
         <v>78.8</v>
       </c>
       <c r="AI32" s="69">
-        <f t="shared" ref="AI32" si="73">IF(OR(ISBLANK(U32), ISBLANK(AB32)),"",U32+AB32)</f>
+        <f t="shared" ref="AI32" si="98">IF(OR(ISBLANK(U32), ISBLANK(AB32)),"",U32+AB32)</f>
         <v>68.873999999999995</v>
       </c>
       <c r="AJ32" s="69" t="str">
-        <f t="shared" ref="AJ32" si="74">IF(OR(ISBLANK(V32), ISBLANK(AC32)),"",V32+AC32)</f>
+        <f t="shared" ref="AJ32" si="99">IF(OR(ISBLANK(V32), ISBLANK(AC32)),"",V32+AC32)</f>
         <v/>
       </c>
       <c r="AK32" s="69" t="str">
-        <f t="shared" ref="AK32" si="75">IF(OR(ISBLANK(W32), ISBLANK(AD32)),"",W32+AD32)</f>
+        <f t="shared" ref="AK32" si="100">IF(OR(ISBLANK(W32), ISBLANK(AD32)),"",W32+AD32)</f>
         <v/>
       </c>
       <c r="AS32" s="61"/>
@@ -7492,9 +7620,7 @@
       <c r="D33" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E33" s="61"/>
       <c r="F33" s="61" t="s">
         <v>142</v>
       </c>
@@ -8002,7 +8128,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A43" sqref="A43"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8031,7 +8157,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>123</v>
@@ -10820,7 +10946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F8BFE4-8461-B541-8467-258963D3527B}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -10864,7 +10990,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>72202</v>
+        <v>99859</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -10882,7 +11008,7 @@
       </c>
       <c r="E3" s="61">
         <f t="shared" ref="E3:E41" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
-        <v>73526</v>
+        <v>57333</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -10900,7 +11026,7 @@
       </c>
       <c r="E4" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>240322</v>
+        <v>155750</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -10918,7 +11044,7 @@
       </c>
       <c r="E5" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>107919</v>
+        <v>90003</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -10936,7 +11062,7 @@
       </c>
       <c r="E6" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>72844</v>
+        <v>100298</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -10954,7 +11080,7 @@
       </c>
       <c r="E7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>92782</v>
+        <v>123657</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -10972,7 +11098,7 @@
       </c>
       <c r="E8" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>92119</v>
+        <v>107777</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10990,7 +11116,7 @@
       </c>
       <c r="E9" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>218353</v>
+        <v>248140</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -11008,7 +11134,7 @@
       </c>
       <c r="E10" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>65475</v>
+        <v>128904</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -11026,7 +11152,7 @@
       </c>
       <c r="E11" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>223699</v>
+        <v>109980</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -11044,7 +11170,7 @@
       </c>
       <c r="E12" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>196417</v>
+        <v>228354</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -11062,7 +11188,7 @@
       </c>
       <c r="E13" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>140770</v>
+        <v>173230</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -11080,7 +11206,7 @@
       </c>
       <c r="E14" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>121912</v>
+        <v>113389</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -11098,7 +11224,7 @@
       </c>
       <c r="E15" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>196880</v>
+        <v>166732</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -11116,7 +11242,7 @@
       </c>
       <c r="E16" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>200429</v>
+        <v>52190</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -11134,7 +11260,7 @@
       </c>
       <c r="E17" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>176914</v>
+        <v>127892</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -11152,7 +11278,7 @@
       </c>
       <c r="E18" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>95469</v>
+        <v>153275</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -11170,7 +11296,7 @@
       </c>
       <c r="E19" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>149405</v>
+        <v>105108</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -11188,7 +11314,7 @@
       </c>
       <c r="E20" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>175462</v>
+        <v>35548</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -11206,7 +11332,7 @@
       </c>
       <c r="E21" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>218599</v>
+        <v>233771</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -11224,7 +11350,7 @@
       </c>
       <c r="E22" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>159201</v>
+        <v>205264</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -11242,7 +11368,7 @@
       </c>
       <c r="E23" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>158753</v>
+        <v>128382</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -11260,7 +11386,7 @@
       </c>
       <c r="E24" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>194641</v>
+        <v>127210</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -11278,7 +11404,7 @@
       </c>
       <c r="E25" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>40914</v>
+        <v>156652</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -11296,7 +11422,7 @@
       </c>
       <c r="E26" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>171655</v>
+        <v>108457</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -11314,7 +11440,7 @@
       </c>
       <c r="E27" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>211491</v>
+        <v>51182</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -11332,7 +11458,7 @@
       </c>
       <c r="E28" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>163760</v>
+        <v>204985</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -11350,7 +11476,7 @@
       </c>
       <c r="E29" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>79169</v>
+        <v>148784</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -11368,7 +11494,7 @@
       </c>
       <c r="E30" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>38383</v>
+        <v>199797</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -11386,7 +11512,7 @@
       </c>
       <c r="E31" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>60079</v>
+        <v>208716</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -11404,7 +11530,7 @@
       </c>
       <c r="E32" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>189840</v>
+        <v>176661</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -11422,7 +11548,7 @@
       </c>
       <c r="E33" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>68380</v>
+        <v>121516</v>
       </c>
     </row>
     <row r="34" spans="1:5">

</xml_diff>

<commit_message>
Add more rows to Sample Data template spreadsheet
Doubled the number of steel companies represented.  Also added some big electrical utilities, including Southern and Xcel.
</commit_message>
<xml_diff>
--- a/examples/data/20220215 ITR Tool Sample Data.xlsx
+++ b/examples/data/20220215 ITR Tool Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC2D88E-09D2-7C45-AFBE-48F94FC59B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F48F7A-FE7B-8F48-B3E0-B60364878D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44680" yWindow="14200" windowWidth="44560" windowHeight="22440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44680" yWindow="14200" windowWidth="44560" windowHeight="22440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -564,12 +564,78 @@
         </r>
       </text>
     </comment>
+    <comment ref="F47" authorId="0" shapeId="0" xr:uid="{B523BD91-66ED-C74B-BC50-E9F5516DC079}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Really S1+S2+S3 but setting to S1+S2 for now.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F52" authorId="0" shapeId="0" xr:uid="{89150159-53A4-8045-B72C-0B04D7E51127}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Really S1+S2+S3 but setting to S1+S2 for now.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2066" uniqueCount="324">
   <si>
     <t>Data field</t>
   </si>
@@ -1673,10 +1739,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1867,23 +1934,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFA6A6A6"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="ArialMT"/>
     </font>
   </fonts>
   <fills count="15">
@@ -2192,10 +2251,10 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3851,13 +3910,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AZ50"/>
+  <dimension ref="A1:AZ52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O13" sqref="O13"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A34:C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -5112,7 +5171,7 @@
         <v>5664119.7339246115</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="16">
+    <row r="12" spans="1:52">
       <c r="A12" s="61" t="s">
         <v>190</v>
       </c>
@@ -5138,7 +5197,7 @@
       <c r="I12" s="5">
         <v>44196</v>
       </c>
-      <c r="J12" s="91">
+      <c r="J12" s="61">
         <v>3210376042</v>
       </c>
       <c r="K12" s="61">
@@ -5176,7 +5235,7 @@
       <c r="AH12" s="69">
         <v>8.448013328</v>
       </c>
-      <c r="AI12" s="89">
+      <c r="AI12" s="88">
         <v>8.448013328</v>
       </c>
       <c r="AS12" s="61">
@@ -5719,7 +5778,7 @@
       <c r="T17" s="2">
         <v>33.246229124999999</v>
       </c>
-      <c r="U17" s="90">
+      <c r="U17" s="89">
         <v>33.246229124999999</v>
       </c>
       <c r="X17" s="2">
@@ -7691,275 +7750,935 @@
       </c>
     </row>
     <row r="34" spans="1:49">
-      <c r="A34" s="61"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="61"/>
-      <c r="L34" s="61"/>
-      <c r="M34" s="61"/>
-      <c r="N34" s="61"/>
-      <c r="P34" s="61"/>
+      <c r="A34" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C34" s="61" t="s">
+        <v>266</v>
+      </c>
+      <c r="D34" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I34" s="5">
+        <v>44196</v>
+      </c>
+      <c r="J34" s="61">
+        <v>8231813171</v>
+      </c>
+      <c r="K34" s="61">
+        <v>3471209000</v>
+      </c>
+      <c r="L34" s="61">
+        <v>14415922171</v>
+      </c>
+      <c r="M34" s="61">
+        <v>14426205171</v>
+      </c>
+      <c r="N34" s="61">
+        <v>18479247000</v>
+      </c>
+      <c r="O34" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P34" s="61" t="s">
+        <v>318</v>
+      </c>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
-      <c r="AS34" s="61"/>
-      <c r="AT34" s="61"/>
-      <c r="AU34" s="61"/>
-      <c r="AV34" s="61"/>
-      <c r="AW34" s="61"/>
+      <c r="AE34" s="69">
+        <v>10.12642009</v>
+      </c>
+      <c r="AF34" s="69">
+        <v>11.12039266</v>
+      </c>
+      <c r="AG34" s="69">
+        <v>11.187042509999999</v>
+      </c>
+      <c r="AH34" s="69">
+        <v>10.54957153</v>
+      </c>
+      <c r="AI34" s="69">
+        <v>10.20926277</v>
+      </c>
+      <c r="AS34" s="61">
+        <v>30.337969149999999</v>
+      </c>
+      <c r="AT34" s="61">
+        <v>31.51282149</v>
+      </c>
+      <c r="AU34" s="61">
+        <v>31.46022512</v>
+      </c>
+      <c r="AV34" s="61">
+        <v>32.008271950000001</v>
+      </c>
+      <c r="AW34" s="61">
+        <v>32.937665989999999</v>
+      </c>
     </row>
     <row r="35" spans="1:49">
-      <c r="A35" s="61"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="61"/>
-      <c r="H35" s="61"/>
-      <c r="J35" s="61"/>
-      <c r="K35" s="61"/>
-      <c r="L35" s="61"/>
-      <c r="M35" s="61"/>
-      <c r="N35" s="61"/>
-      <c r="O35" s="68"/>
-      <c r="P35" s="68"/>
+      <c r="A35" s="61" t="s">
+        <v>267</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C35" s="61" t="s">
+        <v>269</v>
+      </c>
+      <c r="D35" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H35" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I35" s="5">
+        <v>44196</v>
+      </c>
+      <c r="J35" s="61">
+        <v>3725882304</v>
+      </c>
+      <c r="K35" s="61">
+        <v>2123000000</v>
+      </c>
+      <c r="L35" s="61">
+        <v>1</v>
+      </c>
+      <c r="M35" s="61">
+        <v>1</v>
+      </c>
+      <c r="N35" s="61">
+        <v>8394000000</v>
+      </c>
+      <c r="O35" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P35" s="61" t="s">
+        <v>318</v>
+      </c>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
-      <c r="AS35" s="61"/>
-      <c r="AT35" s="61"/>
-      <c r="AU35" s="61"/>
-      <c r="AV35" s="61"/>
-      <c r="AW35" s="61"/>
+      <c r="AE35" s="69">
+        <v>5.9896601059999997</v>
+      </c>
+      <c r="AF35" s="69">
+        <v>5.9839268729999997</v>
+      </c>
+      <c r="AG35" s="69">
+        <v>6.0355401320000004</v>
+      </c>
+      <c r="AH35" s="69">
+        <v>7.6219275870000001</v>
+      </c>
+      <c r="AI35" s="69">
+        <v>7.0609671650000001</v>
+      </c>
+      <c r="AS35" s="61">
+        <v>14.03887716</v>
+      </c>
+      <c r="AT35" s="61">
+        <v>14.15813406</v>
+      </c>
+      <c r="AU35" s="61">
+        <v>14.925387110000001</v>
+      </c>
+      <c r="AV35" s="61">
+        <v>16.800690790000001</v>
+      </c>
+      <c r="AW35" s="61">
+        <v>16.963449130000001</v>
+      </c>
     </row>
     <row r="36" spans="1:49">
-      <c r="A36" s="61"/>
-      <c r="C36" s="61"/>
-      <c r="D36" s="61"/>
-      <c r="E36" s="61"/>
-      <c r="F36" s="61"/>
-      <c r="H36" s="61"/>
-      <c r="J36" s="61"/>
-      <c r="K36" s="61"/>
-      <c r="L36" s="61"/>
-      <c r="M36" s="61"/>
-      <c r="N36" s="61"/>
-      <c r="O36" s="68"/>
-      <c r="P36" s="68"/>
+      <c r="A36" s="61" t="s">
+        <v>270</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C36" s="61" t="s">
+        <v>272</v>
+      </c>
+      <c r="D36" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I36" s="5">
+        <v>44196</v>
+      </c>
+      <c r="J36" s="61">
+        <v>24648067675</v>
+      </c>
+      <c r="K36" s="61">
+        <v>10076000000</v>
+      </c>
+      <c r="L36" s="61">
+        <v>41224067675</v>
+      </c>
+      <c r="M36" s="61">
+        <v>41371067675</v>
+      </c>
+      <c r="N36" s="61">
+        <v>47730000000</v>
+      </c>
+      <c r="O36" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P36" s="61" t="s">
+        <v>318</v>
+      </c>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
-      <c r="AS36" s="61"/>
-      <c r="AT36" s="61"/>
-      <c r="AU36" s="61"/>
-      <c r="AV36" s="61"/>
-      <c r="AW36" s="61"/>
+      <c r="AE36" s="69">
+        <v>11.512385626</v>
+      </c>
+      <c r="AF36" s="69">
+        <v>10.497904363</v>
+      </c>
+      <c r="AG36" s="69">
+        <v>11.887135768</v>
+      </c>
+      <c r="AH36" s="69">
+        <v>11.572505309</v>
+      </c>
+      <c r="AI36" s="69">
+        <v>0</v>
+      </c>
+      <c r="AS36" s="61">
+        <v>53.073391780000001</v>
+      </c>
+      <c r="AT36" s="61">
+        <v>52.677105660000002</v>
+      </c>
+      <c r="AU36" s="61">
+        <v>55.323284050000012</v>
+      </c>
+      <c r="AV36" s="61">
+        <v>54.987423449999987</v>
+      </c>
+      <c r="AW36" s="61">
+        <v>50.81882119748181</v>
+      </c>
     </row>
     <row r="37" spans="1:49">
-      <c r="A37" s="61"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="61"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="61"/>
-      <c r="H37" s="61"/>
-      <c r="J37" s="61"/>
-      <c r="K37" s="61"/>
-      <c r="L37" s="61"/>
-      <c r="M37" s="61"/>
-      <c r="N37" s="61"/>
-      <c r="O37" s="68"/>
-      <c r="P37" s="68"/>
+      <c r="A37" s="61" t="s">
+        <v>276</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C37" s="61" t="s">
+        <v>278</v>
+      </c>
+      <c r="D37" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H37" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I37" s="5">
+        <v>44196</v>
+      </c>
+      <c r="J37" s="61">
+        <v>34300000000</v>
+      </c>
+      <c r="K37" s="61">
+        <v>10829000000</v>
+      </c>
+      <c r="L37" s="61">
+        <v>54977000000</v>
+      </c>
+      <c r="M37" s="61">
+        <v>55085000000</v>
+      </c>
+      <c r="N37" s="61">
+        <v>65665000000</v>
+      </c>
+      <c r="O37" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P37" s="61" t="s">
+        <v>318</v>
+      </c>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
-      <c r="AS37" s="61"/>
-      <c r="AT37" s="61"/>
-      <c r="AU37" s="61"/>
-      <c r="AV37" s="61"/>
-      <c r="AW37" s="61"/>
+      <c r="AE37" s="69">
+        <v>0.93325630999999998</v>
+      </c>
+      <c r="AF37" s="69">
+        <v>1.0145733539999999</v>
+      </c>
+      <c r="AG37" s="69">
+        <v>0.78712423499999995</v>
+      </c>
+      <c r="AH37" s="69">
+        <v>0.49535753599999999</v>
+      </c>
+      <c r="AI37" s="69">
+        <v>0.476305323</v>
+      </c>
+      <c r="AS37" s="61">
+        <v>7.0559976339999997</v>
+      </c>
+      <c r="AT37" s="61">
+        <v>7.7571735559999997</v>
+      </c>
+      <c r="AU37" s="61">
+        <v>7.5840753850000002</v>
+      </c>
+      <c r="AV37" s="61">
+        <v>7.0361163089999996</v>
+      </c>
+      <c r="AW37" s="61">
+        <v>6.5027076047105936</v>
+      </c>
     </row>
     <row r="38" spans="1:49">
-      <c r="A38" s="61"/>
-      <c r="C38" s="61"/>
-      <c r="D38" s="61"/>
-      <c r="E38" s="61"/>
-      <c r="F38" s="61"/>
-      <c r="H38" s="61"/>
-      <c r="J38" s="61"/>
-      <c r="K38" s="61"/>
-      <c r="L38" s="61"/>
-      <c r="M38" s="61"/>
-      <c r="N38" s="61"/>
-      <c r="O38" s="68"/>
-      <c r="P38" s="68"/>
+      <c r="A38" s="61" t="s">
+        <v>279</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C38" s="61" t="s">
+        <v>281</v>
+      </c>
+      <c r="D38" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H38" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I38" s="5">
+        <v>44196</v>
+      </c>
+      <c r="J38" s="61">
+        <v>54800000000</v>
+      </c>
+      <c r="K38" s="61">
+        <v>22596000000</v>
+      </c>
+      <c r="L38" s="61">
+        <v>94623000000</v>
+      </c>
+      <c r="M38" s="61">
+        <v>96598000000</v>
+      </c>
+      <c r="N38" s="61">
+        <v>118700000000</v>
+      </c>
+      <c r="O38" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P38" s="61" t="s">
+        <v>318</v>
+      </c>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
-      <c r="AS38" s="61"/>
-      <c r="AT38" s="61"/>
-      <c r="AU38" s="61"/>
-      <c r="AV38" s="61"/>
-      <c r="AW38" s="61"/>
+      <c r="AE38" s="69">
+        <v>76.819825894000004</v>
+      </c>
+      <c r="AF38" s="69">
+        <v>68.689750579000005</v>
+      </c>
+      <c r="AG38" s="69">
+        <v>70.065115272</v>
+      </c>
+      <c r="AH38" s="69">
+        <v>63.436548403000003</v>
+      </c>
+      <c r="AI38" s="69">
+        <v>63.538943889999999</v>
+      </c>
+      <c r="AS38" s="61">
+        <v>147.55628282000001</v>
+      </c>
+      <c r="AT38" s="61">
+        <v>144.79387678000001</v>
+      </c>
+      <c r="AU38" s="61">
+        <v>149.25604005</v>
+      </c>
+      <c r="AV38" s="61">
+        <v>145.52973376</v>
+      </c>
+      <c r="AW38" s="61">
+        <v>134.49710960891679</v>
+      </c>
     </row>
     <row r="39" spans="1:49">
-      <c r="A39" s="61"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="61"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="61"/>
-      <c r="H39" s="61"/>
-      <c r="J39" s="61"/>
-      <c r="K39" s="61"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="61"/>
-      <c r="N39" s="61"/>
-      <c r="P39" s="61"/>
+      <c r="A39" s="61" t="s">
+        <v>273</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C39" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="D39" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="61" t="s">
+        <v>182</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I39" s="5">
+        <v>44196</v>
+      </c>
+      <c r="J39" s="61">
+        <v>4100000000</v>
+      </c>
+      <c r="K39" s="61">
+        <v>10464991000</v>
+      </c>
+      <c r="L39" s="61">
+        <v>5452884000</v>
+      </c>
+      <c r="M39" s="61">
+        <v>6834344000</v>
+      </c>
+      <c r="N39" s="61">
+        <v>8275765000</v>
+      </c>
+      <c r="O39" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P39" s="61" t="s">
+        <v>320</v>
+      </c>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
-      <c r="AS39" s="61"/>
-      <c r="AT39" s="61"/>
-      <c r="AU39" s="61"/>
-      <c r="AV39" s="61"/>
-      <c r="AW39" s="61"/>
+      <c r="AE39" s="69">
+        <v>4.9161869999999999</v>
+      </c>
+      <c r="AF39" s="69">
+        <v>4.9161869999999999</v>
+      </c>
+      <c r="AG39" s="69">
+        <v>5.162928</v>
+      </c>
+      <c r="AH39" s="69">
+        <v>4.8897659999999998</v>
+      </c>
+      <c r="AI39" s="69">
+        <v>4.8618244799999983</v>
+      </c>
+      <c r="AS39" s="61">
+        <v>9.4542057692307679</v>
+      </c>
+      <c r="AT39" s="61">
+        <v>9.4542057692307679</v>
+      </c>
+      <c r="AU39" s="61">
+        <v>9.7413735849056593</v>
+      </c>
+      <c r="AV39" s="61">
+        <v>9.9791142857142852</v>
+      </c>
+      <c r="AW39" s="61">
+        <v>10.128800999999999</v>
+      </c>
     </row>
     <row r="40" spans="1:49">
-      <c r="A40" s="61"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="61"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="61"/>
-      <c r="H40" s="61"/>
+      <c r="A40" s="61" t="s">
+        <v>282</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C40" s="61" t="s">
+        <v>284</v>
+      </c>
+      <c r="D40" s="61" t="s">
+        <v>154</v>
+      </c>
+      <c r="E40" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I40" s="5">
+        <v>44196</v>
+      </c>
       <c r="J40" s="61"/>
-      <c r="K40" s="61"/>
-      <c r="L40" s="61"/>
-      <c r="M40" s="61"/>
-      <c r="N40" s="61"/>
-      <c r="O40" s="68"/>
-      <c r="P40" s="68"/>
+      <c r="K40" s="61">
+        <v>10166444011.05982</v>
+      </c>
+      <c r="L40" s="61">
+        <v>1</v>
+      </c>
+      <c r="M40" s="61">
+        <v>1</v>
+      </c>
+      <c r="N40" s="61">
+        <v>76145937002.942871</v>
+      </c>
+      <c r="O40" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P40" s="61" t="s">
+        <v>318</v>
+      </c>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
-      <c r="AS40" s="61"/>
-      <c r="AT40" s="61"/>
-      <c r="AU40" s="61"/>
-      <c r="AV40" s="61"/>
-      <c r="AW40" s="61"/>
+      <c r="AE40" s="69">
+        <v>0.37608664600000002</v>
+      </c>
+      <c r="AF40" s="69">
+        <v>0.47113547300000003</v>
+      </c>
+      <c r="AG40" s="69">
+        <v>0.71664363799999997</v>
+      </c>
+      <c r="AH40" s="69">
+        <v>0.58371024299999996</v>
+      </c>
+      <c r="AI40" s="69">
+        <v>0</v>
+      </c>
+      <c r="AS40" s="61">
+        <v>0.77214899999999997</v>
+      </c>
+      <c r="AT40" s="61">
+        <v>1.0567139999999999</v>
+      </c>
+      <c r="AU40" s="61">
+        <v>1.51502</v>
+      </c>
+      <c r="AV40" s="61">
+        <v>1.2483029999999999</v>
+      </c>
+      <c r="AW40" s="61">
+        <v>1.153669020607295</v>
+      </c>
     </row>
     <row r="41" spans="1:49">
-      <c r="A41" s="61"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="H41" s="61"/>
+      <c r="A41" s="61" t="s">
+        <v>285</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C41" s="61" t="s">
+        <v>287</v>
+      </c>
+      <c r="D41" s="61" t="s">
+        <v>288</v>
+      </c>
+      <c r="E41" s="61" t="s">
+        <v>241</v>
+      </c>
+      <c r="F41" s="61" t="s">
+        <v>182</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H41" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I41" s="5">
+        <v>44196</v>
+      </c>
       <c r="J41" s="61"/>
-      <c r="K41" s="61"/>
-      <c r="L41" s="61"/>
-      <c r="M41" s="61"/>
-      <c r="N41" s="61"/>
-      <c r="O41" s="68"/>
-      <c r="P41" s="68"/>
+      <c r="K41" s="61">
+        <v>7294055000</v>
+      </c>
+      <c r="L41" s="61">
+        <v>1</v>
+      </c>
+      <c r="M41" s="61">
+        <v>1</v>
+      </c>
+      <c r="N41" s="61">
+        <v>14842991000</v>
+      </c>
+      <c r="O41" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P41" s="61" t="s">
+        <v>320</v>
+      </c>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
-      <c r="AS41" s="61"/>
-      <c r="AT41" s="61"/>
-      <c r="AU41" s="61"/>
-      <c r="AV41" s="61"/>
-      <c r="AW41" s="61"/>
+      <c r="AE41" s="69">
+        <v>2.9</v>
+      </c>
+      <c r="AF41" s="69">
+        <v>2.9</v>
+      </c>
+      <c r="AG41" s="69">
+        <v>2.9</v>
+      </c>
+      <c r="AH41" s="69">
+        <v>2.7</v>
+      </c>
+      <c r="AI41" s="69">
+        <v>1.5</v>
+      </c>
+      <c r="AS41" s="61">
+        <v>3.933333333333334</v>
+      </c>
+      <c r="AT41" s="61">
+        <v>3.933333333333334</v>
+      </c>
+      <c r="AU41" s="61">
+        <v>3.933333333333334</v>
+      </c>
+      <c r="AV41" s="61">
+        <v>3.5</v>
+      </c>
+      <c r="AW41" s="61">
+        <v>2.1538461538461542</v>
+      </c>
     </row>
     <row r="42" spans="1:49">
-      <c r="A42" s="61"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="61"/>
-      <c r="H42" s="61"/>
-      <c r="J42" s="61"/>
-      <c r="K42" s="61"/>
-      <c r="L42" s="61"/>
-      <c r="M42" s="61"/>
-      <c r="N42" s="61"/>
-      <c r="O42" s="68"/>
-      <c r="P42" s="68"/>
+      <c r="A42" s="61" t="s">
+        <v>289</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C42" s="61" t="s">
+        <v>291</v>
+      </c>
+      <c r="D42" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" s="61" t="s">
+        <v>182</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H42" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I42" s="5">
+        <v>44196</v>
+      </c>
+      <c r="J42" s="61">
+        <v>160935221</v>
+      </c>
+      <c r="K42" s="61">
+        <v>1208800000</v>
+      </c>
+      <c r="L42" s="61">
+        <v>302435221</v>
+      </c>
+      <c r="M42" s="61">
+        <v>329535221</v>
+      </c>
+      <c r="N42" s="61">
+        <v>1085200000</v>
+      </c>
+      <c r="O42" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P42" s="61" t="s">
+        <v>320</v>
+      </c>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
-      <c r="AS42" s="61"/>
-      <c r="AT42" s="61"/>
-      <c r="AU42" s="61"/>
-      <c r="AV42" s="61"/>
-      <c r="AW42" s="61"/>
+      <c r="AE42" s="69">
+        <v>0.42172199999999999</v>
+      </c>
+      <c r="AF42" s="69">
+        <v>0.42172199999999999</v>
+      </c>
+      <c r="AG42" s="69">
+        <v>0.42172199999999999</v>
+      </c>
+      <c r="AH42" s="69">
+        <v>0.29852600000000001</v>
+      </c>
+      <c r="AI42" s="69">
+        <v>0.197605</v>
+      </c>
+      <c r="AS42" s="61">
+        <v>1.415411</v>
+      </c>
+      <c r="AT42" s="61">
+        <v>1.415411</v>
+      </c>
+      <c r="AU42" s="61">
+        <v>1.415411</v>
+      </c>
+      <c r="AV42" s="61">
+        <v>0.96435300000000002</v>
+      </c>
+      <c r="AW42" s="61">
+        <v>0.65796399999999999</v>
+      </c>
     </row>
     <row r="43" spans="1:49">
-      <c r="A43" s="61"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="61"/>
-      <c r="H43" s="61"/>
-      <c r="J43" s="61"/>
-      <c r="K43" s="61"/>
-      <c r="L43" s="61"/>
-      <c r="M43" s="61"/>
-      <c r="N43" s="61"/>
-      <c r="P43" s="61"/>
+      <c r="A43" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C43" s="61" t="s">
+        <v>294</v>
+      </c>
+      <c r="D43" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" s="61" t="s">
+        <v>182</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H43" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I43" s="5">
+        <v>44196</v>
+      </c>
+      <c r="J43" s="61">
+        <v>1600000000</v>
+      </c>
+      <c r="K43" s="61">
+        <v>12937000000</v>
+      </c>
+      <c r="L43" s="61">
+        <v>4630000000</v>
+      </c>
+      <c r="M43" s="61">
+        <v>5379000000</v>
+      </c>
+      <c r="N43" s="61">
+        <v>11608000000</v>
+      </c>
+      <c r="O43" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P43" s="61" t="s">
+        <v>320</v>
+      </c>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
-      <c r="AS43" s="61"/>
-      <c r="AT43" s="61"/>
-      <c r="AU43" s="61"/>
-      <c r="AV43" s="61"/>
-      <c r="AW43" s="61"/>
+      <c r="AE43" s="69">
+        <v>32.421599999999998</v>
+      </c>
+      <c r="AF43" s="69">
+        <v>33.067599999999999</v>
+      </c>
+      <c r="AG43" s="69">
+        <v>35.458500000000001</v>
+      </c>
+      <c r="AH43" s="69">
+        <v>33.058199999999999</v>
+      </c>
+      <c r="AI43" s="69">
+        <v>27.003599999999999</v>
+      </c>
+      <c r="AS43" s="61">
+        <v>14.22</v>
+      </c>
+      <c r="AT43" s="61">
+        <v>14.44</v>
+      </c>
+      <c r="AU43" s="61">
+        <v>15.35</v>
+      </c>
+      <c r="AV43" s="61">
+        <v>13.89</v>
+      </c>
+      <c r="AW43" s="61">
+        <v>11.54</v>
+      </c>
     </row>
     <row r="44" spans="1:49">
-      <c r="A44" s="61"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="61"/>
-      <c r="F44" s="61"/>
-      <c r="H44" s="61"/>
-      <c r="J44" s="61"/>
-      <c r="K44" s="61"/>
-      <c r="L44" s="61"/>
-      <c r="M44" s="61"/>
-      <c r="N44" s="61"/>
-      <c r="P44" s="61"/>
+      <c r="A44" s="61" t="s">
+        <v>307</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C44" s="61" t="s">
+        <v>309</v>
+      </c>
+      <c r="D44" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F44" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H44" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I44" s="5">
+        <v>44196</v>
+      </c>
+      <c r="J44" s="61">
+        <v>32825311125</v>
+      </c>
+      <c r="K44" s="61">
+        <v>11529000000</v>
+      </c>
+      <c r="L44" s="61">
+        <v>1</v>
+      </c>
+      <c r="M44" s="61">
+        <v>1</v>
+      </c>
+      <c r="N44" s="61">
+        <v>50448000000</v>
+      </c>
+      <c r="O44" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P44" s="61" t="s">
+        <v>318</v>
+      </c>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
-      <c r="AS44" s="61"/>
-      <c r="AT44" s="61"/>
-      <c r="AU44" s="61"/>
-      <c r="AV44" s="61"/>
-      <c r="AW44" s="61"/>
+      <c r="AE44" s="69">
+        <v>46.128179090000003</v>
+      </c>
+      <c r="AF44" s="69">
+        <v>44.807197789999996</v>
+      </c>
+      <c r="AG44" s="69">
+        <v>47.025298190000001</v>
+      </c>
+      <c r="AH44" s="69">
+        <v>43.15126858</v>
+      </c>
+      <c r="AI44" s="69">
+        <v>40.042084060000001</v>
+      </c>
+      <c r="AS44" s="61">
+        <v>88.456566530000003</v>
+      </c>
+      <c r="AT44" s="61">
+        <v>86.887076559999997</v>
+      </c>
+      <c r="AU44" s="61">
+        <v>91.462663679999991</v>
+      </c>
+      <c r="AV44" s="61">
+        <v>92.205090630000001</v>
+      </c>
+      <c r="AW44" s="61">
+        <v>92.771096270000001</v>
+      </c>
     </row>
     <row r="45" spans="1:49">
       <c r="A45" s="61"/>
@@ -7997,8 +8716,7 @@
       <c r="L46" s="61"/>
       <c r="M46" s="61"/>
       <c r="N46" s="61"/>
-      <c r="O46" s="68"/>
-      <c r="P46" s="68"/>
+      <c r="P46" s="61"/>
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
       <c r="S46" s="2"/>
@@ -8022,8 +8740,7 @@
       <c r="L47" s="61"/>
       <c r="M47" s="61"/>
       <c r="N47" s="61"/>
-      <c r="O47" s="68"/>
-      <c r="P47" s="68"/>
+      <c r="P47" s="61"/>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
       <c r="S47" s="2"/>
@@ -8072,7 +8789,8 @@
       <c r="L49" s="61"/>
       <c r="M49" s="61"/>
       <c r="N49" s="61"/>
-      <c r="P49" s="61"/>
+      <c r="O49" s="68"/>
+      <c r="P49" s="68"/>
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
       <c r="S49" s="2"/>
@@ -8109,6 +8827,55 @@
       <c r="AV50" s="61"/>
       <c r="AW50" s="61"/>
     </row>
+    <row r="51" spans="1:49">
+      <c r="A51" s="61"/>
+      <c r="C51" s="61"/>
+      <c r="D51" s="61"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="61"/>
+      <c r="H51" s="61"/>
+      <c r="J51" s="61"/>
+      <c r="K51" s="61"/>
+      <c r="L51" s="61"/>
+      <c r="M51" s="61"/>
+      <c r="N51" s="61"/>
+      <c r="P51" s="61"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+      <c r="S51" s="2"/>
+      <c r="T51" s="2"/>
+      <c r="U51" s="2"/>
+      <c r="AS51" s="61"/>
+      <c r="AT51" s="61"/>
+      <c r="AU51" s="61"/>
+      <c r="AV51" s="61"/>
+      <c r="AW51" s="61"/>
+    </row>
+    <row r="52" spans="1:49">
+      <c r="A52" s="61"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="61"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="61"/>
+      <c r="H52" s="61"/>
+      <c r="J52" s="61"/>
+      <c r="K52" s="61"/>
+      <c r="L52" s="61"/>
+      <c r="M52" s="61"/>
+      <c r="N52" s="61"/>
+      <c r="O52" s="68"/>
+      <c r="P52" s="68"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="2"/>
+      <c r="U52" s="2"/>
+      <c r="AS52" s="61"/>
+      <c r="AT52" s="61"/>
+      <c r="AU52" s="61"/>
+      <c r="AV52" s="61"/>
+      <c r="AW52" s="61"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8122,13 +8889,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AEF12C-8FCA-4C98-A7E3-A92507F3829D}">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9706,25 +10473,451 @@
       </c>
     </row>
     <row r="44" spans="1:12">
-      <c r="I44" s="76"/>
+      <c r="A44" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C44" s="61" t="s">
+        <v>266</v>
+      </c>
+      <c r="D44" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E44" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F44" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G44" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H44" s="20">
+        <v>2005</v>
+      </c>
+      <c r="I44" s="90">
+        <v>16557441</v>
+      </c>
+      <c r="J44" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="K44" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L44" s="75">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="45" spans="1:12">
-      <c r="I45" s="76"/>
+      <c r="A45" s="61" t="s">
+        <v>267</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C45" s="61" t="s">
+        <v>269</v>
+      </c>
+      <c r="D45" s="26">
+        <v>2040</v>
+      </c>
+      <c r="E45" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F45" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G45" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H45" s="20">
+        <v>2010</v>
+      </c>
+      <c r="I45" s="61">
+        <v>0.47</v>
+      </c>
+      <c r="J45" s="61" t="s">
+        <v>317</v>
+      </c>
+      <c r="K45" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L45" s="75">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="46" spans="1:12">
-      <c r="I46" s="76"/>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="I47" s="76"/>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="I48" s="76"/>
-    </row>
-    <row r="49" spans="9:9">
-      <c r="I49" s="76"/>
-    </row>
-    <row r="50" spans="9:9">
-      <c r="I50" s="76"/>
+      <c r="A46" s="61" t="s">
+        <v>270</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C46" s="61" t="s">
+        <v>272</v>
+      </c>
+      <c r="D46" s="26">
+        <v>2030</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F46" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G46" s="61">
+        <v>2021</v>
+      </c>
+      <c r="H46" s="20">
+        <v>2005</v>
+      </c>
+      <c r="I46" s="76">
+        <v>26566330</v>
+      </c>
+      <c r="J46" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="K46" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L46" s="75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="61" customFormat="1">
+      <c r="A47" s="61" t="s">
+        <v>276</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C47" s="61" t="s">
+        <v>278</v>
+      </c>
+      <c r="D47" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F47" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G47" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H47" s="20">
+        <v>2019</v>
+      </c>
+      <c r="I47" s="91">
+        <v>0.80243130614229874</v>
+      </c>
+      <c r="J47" s="61" t="s">
+        <v>317</v>
+      </c>
+      <c r="K47" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L47" s="75">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="61" customFormat="1">
+      <c r="A48" s="61" t="s">
+        <v>279</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C48" s="61" t="s">
+        <v>281</v>
+      </c>
+      <c r="D48" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F48" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G48" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H48" s="20">
+        <v>2007</v>
+      </c>
+      <c r="I48" s="91">
+        <v>0.98420553538837829</v>
+      </c>
+      <c r="J48" s="61" t="s">
+        <v>317</v>
+      </c>
+      <c r="K48" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L48" s="75">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="61" t="s">
+        <v>273</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C49" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="D49" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E49" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F49" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G49" s="61">
+        <v>2021</v>
+      </c>
+      <c r="H49" s="20">
+        <v>2018</v>
+      </c>
+      <c r="I49" s="61">
+        <v>5.162928</v>
+      </c>
+      <c r="J49" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="K49" s="61">
+        <v>2025</v>
+      </c>
+      <c r="L49" s="75">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="61" customFormat="1">
+      <c r="A50" s="61" t="s">
+        <v>273</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C50" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="D50" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F50" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G50" s="61">
+        <v>2021</v>
+      </c>
+      <c r="H50" s="20">
+        <v>2018</v>
+      </c>
+      <c r="I50" s="61">
+        <v>5.162928</v>
+      </c>
+      <c r="J50" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="K50" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L50" s="75">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="61" t="s">
+        <v>282</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C51" s="61" t="s">
+        <v>284</v>
+      </c>
+      <c r="D51" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F51" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G51" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H51" s="20">
+        <v>2019</v>
+      </c>
+      <c r="I51" s="91">
+        <v>0.46760301224942979</v>
+      </c>
+      <c r="J51" s="61" t="s">
+        <v>317</v>
+      </c>
+      <c r="K51" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L51" s="75">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="61" t="s">
+        <v>285</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C52" s="61" t="s">
+        <v>287</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F52" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G52" s="61">
+        <v>2021</v>
+      </c>
+      <c r="H52" s="20">
+        <v>2018</v>
+      </c>
+      <c r="I52" s="91">
+        <v>2.9</v>
+      </c>
+      <c r="J52" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="K52" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L52" s="75">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="61" t="s">
+        <v>289</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C53" s="61" t="s">
+        <v>291</v>
+      </c>
+      <c r="E53" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F53" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G53" s="61">
+        <v>2021</v>
+      </c>
+      <c r="H53" s="20">
+        <v>2018</v>
+      </c>
+      <c r="I53" s="91">
+        <v>0.42172199999999999</v>
+      </c>
+      <c r="J53" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="K53" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L53" s="75">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C54" s="61" t="s">
+        <v>294</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F54" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G54" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H54" s="20">
+        <v>2018</v>
+      </c>
+      <c r="I54" s="91">
+        <v>0.315911</v>
+      </c>
+      <c r="J54" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="K54" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L54" s="75">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="61" t="s">
+        <v>307</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C55" s="61" t="s">
+        <v>309</v>
+      </c>
+      <c r="D55" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E55" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F55" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G55" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H55" s="20">
+        <v>2005</v>
+      </c>
+      <c r="I55" s="91">
+        <v>0.88086205923584682</v>
+      </c>
+      <c r="J55" s="61" t="s">
+        <v>317</v>
+      </c>
+      <c r="K55" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L55" s="75">
+        <v>0.8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10944,10 +12137,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F8BFE4-8461-B541-8467-258963D3527B}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10990,7 +12183,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>99859</v>
+        <v>178650</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -11007,8 +12200,8 @@
         <v>147</v>
       </c>
       <c r="E3" s="61">
-        <f t="shared" ref="E3:E41" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
-        <v>57333</v>
+        <f t="shared" ref="E3:E44" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
+        <v>126908</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -11026,7 +12219,7 @@
       </c>
       <c r="E4" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>155750</v>
+        <v>175844</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -11044,7 +12237,7 @@
       </c>
       <c r="E5" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>90003</v>
+        <v>244845</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -11062,7 +12255,7 @@
       </c>
       <c r="E6" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>100298</v>
+        <v>126020</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -11080,7 +12273,7 @@
       </c>
       <c r="E7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>123657</v>
+        <v>103176</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -11098,7 +12291,7 @@
       </c>
       <c r="E8" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>107777</v>
+        <v>167980</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -11116,7 +12309,7 @@
       </c>
       <c r="E9" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>248140</v>
+        <v>245505</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -11134,7 +12327,7 @@
       </c>
       <c r="E10" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>128904</v>
+        <v>216265</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -11152,7 +12345,7 @@
       </c>
       <c r="E11" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>109980</v>
+        <v>173275</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -11170,7 +12363,7 @@
       </c>
       <c r="E12" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>228354</v>
+        <v>67366</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -11188,7 +12381,7 @@
       </c>
       <c r="E13" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>173230</v>
+        <v>120343</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -11206,7 +12399,7 @@
       </c>
       <c r="E14" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>113389</v>
+        <v>70900</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -11224,7 +12417,7 @@
       </c>
       <c r="E15" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>166732</v>
+        <v>122450</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -11242,7 +12435,7 @@
       </c>
       <c r="E16" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>52190</v>
+        <v>235297</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -11260,7 +12453,7 @@
       </c>
       <c r="E17" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>127892</v>
+        <v>84691</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -11278,7 +12471,7 @@
       </c>
       <c r="E18" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>153275</v>
+        <v>206841</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -11296,7 +12489,7 @@
       </c>
       <c r="E19" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>105108</v>
+        <v>77352</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -11314,7 +12507,7 @@
       </c>
       <c r="E20" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>35548</v>
+        <v>138084</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -11332,7 +12525,7 @@
       </c>
       <c r="E21" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>233771</v>
+        <v>99654</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -11350,7 +12543,7 @@
       </c>
       <c r="E22" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>205264</v>
+        <v>186876</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -11368,7 +12561,7 @@
       </c>
       <c r="E23" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>128382</v>
+        <v>222695</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -11386,7 +12579,7 @@
       </c>
       <c r="E24" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>127210</v>
+        <v>152722</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -11404,7 +12597,7 @@
       </c>
       <c r="E25" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>156652</v>
+        <v>118091</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -11422,7 +12615,7 @@
       </c>
       <c r="E26" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>108457</v>
+        <v>60678</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -11440,7 +12633,7 @@
       </c>
       <c r="E27" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>51182</v>
+        <v>224757</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -11458,7 +12651,7 @@
       </c>
       <c r="E28" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>204985</v>
+        <v>191542</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -11476,7 +12669,7 @@
       </c>
       <c r="E29" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>148784</v>
+        <v>191539</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -11494,7 +12687,7 @@
       </c>
       <c r="E30" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>199797</v>
+        <v>104513</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -11512,7 +12705,7 @@
       </c>
       <c r="E31" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>208716</v>
+        <v>245280</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -11530,7 +12723,7 @@
       </c>
       <c r="E32" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>176661</v>
+        <v>174558</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -11548,64 +12741,206 @@
       </c>
       <c r="E33" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>121516</v>
+        <v>126189</v>
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="68"/>
-      <c r="B34" s="88"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="61"/>
+      <c r="A34" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C34" s="61" t="s">
+        <v>266</v>
+      </c>
+      <c r="D34" s="61" t="s">
+        <v>266</v>
+      </c>
+      <c r="E34" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>123996</v>
+      </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="68"/>
-      <c r="B35" s="88"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="61"/>
+      <c r="A35" s="61" t="s">
+        <v>267</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C35" s="61" t="s">
+        <v>269</v>
+      </c>
+      <c r="D35" s="61" t="s">
+        <v>269</v>
+      </c>
+      <c r="E35" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>138805</v>
+      </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="68"/>
-      <c r="B36" s="88"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="61"/>
+      <c r="A36" s="61" t="s">
+        <v>270</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C36" s="61" t="s">
+        <v>272</v>
+      </c>
+      <c r="D36" s="61" t="s">
+        <v>272</v>
+      </c>
+      <c r="E36" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>227679</v>
+      </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="68"/>
-      <c r="B37" s="88"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="61"/>
+      <c r="A37" s="61" t="s">
+        <v>276</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C37" s="61" t="s">
+        <v>278</v>
+      </c>
+      <c r="D37" s="61" t="s">
+        <v>278</v>
+      </c>
+      <c r="E37" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>198758</v>
+      </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="68"/>
-      <c r="B38" s="88"/>
-      <c r="C38" s="68"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="61"/>
+      <c r="A38" s="61" t="s">
+        <v>279</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C38" s="61" t="s">
+        <v>281</v>
+      </c>
+      <c r="D38" s="61" t="s">
+        <v>281</v>
+      </c>
+      <c r="E38" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>102749</v>
+      </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="68"/>
-      <c r="B39" s="88"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="61"/>
+      <c r="A39" s="61" t="s">
+        <v>273</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C39" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="D39" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="E39" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>38693</v>
+      </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="68"/>
-      <c r="B40" s="88"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="61"/>
+      <c r="A40" s="61" t="s">
+        <v>282</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C40" s="61" t="s">
+        <v>284</v>
+      </c>
+      <c r="D40" s="61" t="s">
+        <v>284</v>
+      </c>
+      <c r="E40" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>195002</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="68"/>
-      <c r="B41" s="88"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="61"/>
+      <c r="A41" s="61" t="s">
+        <v>285</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C41" s="61" t="s">
+        <v>287</v>
+      </c>
+      <c r="D41" s="61" t="s">
+        <v>287</v>
+      </c>
+      <c r="E41" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>204355</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="61" t="s">
+        <v>289</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C42" s="61" t="s">
+        <v>291</v>
+      </c>
+      <c r="D42" s="61" t="s">
+        <v>291</v>
+      </c>
+      <c r="E42" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>57497</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C43" s="61" t="s">
+        <v>294</v>
+      </c>
+      <c r="D43" s="61" t="s">
+        <v>294</v>
+      </c>
+      <c r="E43" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>120912</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="61" t="s">
+        <v>307</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C44" s="61" t="s">
+        <v>309</v>
+      </c>
+      <c r="D44" s="61" t="s">
+        <v>309</v>
+      </c>
+      <c r="E44" s="61">
+        <f t="shared" ca="1" si="0"/>
+        <v>79304</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11620,10 +12955,10 @@
   <dimension ref="A1:AZ54"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A40" sqref="A40:XFD40"/>
+      <selection pane="bottomRight" activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -16243,8 +17578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B625E0-7A95-AB40-9EC5-2C6C2025FC51}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Adding check for sectors in scope while reading xlsx with input data
Signed-off-by: oleksandr-anufriyev1 <oleksandr.anufriyev1@allianz.com>
Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data/20220215 ITR Tool Sample Data.xlsx
+++ b/examples/data/20220215 ITR Tool Sample Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/test/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\FC\DSI\Team\Sasha\sasha_code\ITR_develop\examples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F48F7A-FE7B-8F48-B3E0-B60364878D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF6CE08-254D-4C25-812B-92D38941D60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44680" yWindow="14200" windowWidth="44560" windowHeight="22440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -1741,7 +1741,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -2254,10 +2254,10 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3165,7 +3165,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3465,7 +3465,7 @@
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="20" spans="12:18">
       <c r="L20" s="2"/>
@@ -3494,9 +3494,9 @@
       <selection activeCell="AN14" sqref="AN13:AN14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:52" s="3" customFormat="1" ht="16">
+    <row r="1" spans="1:52" s="3" customFormat="1" ht="28.8">
       <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
@@ -3811,6 +3811,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000Confidential&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3822,7 +3826,7 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:12" s="61" customFormat="1">
       <c r="A1" s="10" t="s">
@@ -3902,6 +3906,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000Confidential&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3912,34 +3920,34 @@
   </sheetPr>
   <dimension ref="A1:AZ52"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A34" sqref="A34:C44"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="24"/>
-    <col min="7" max="7" width="16.5" style="4"/>
-    <col min="9" max="9" width="16.5" style="5"/>
-    <col min="14" max="14" width="25.83203125" customWidth="1"/>
-    <col min="15" max="15" width="25.83203125" style="61" customWidth="1"/>
-    <col min="16" max="16" width="22.1640625" customWidth="1"/>
-    <col min="17" max="21" width="16.5" customWidth="1"/>
-    <col min="22" max="22" width="16.5" style="2" customWidth="1"/>
-    <col min="23" max="23" width="16.5" style="36" customWidth="1"/>
-    <col min="24" max="29" width="16.5" style="2" customWidth="1"/>
-    <col min="30" max="30" width="16.5" style="36" customWidth="1"/>
-    <col min="31" max="37" width="16.5" style="2" customWidth="1"/>
-    <col min="38" max="44" width="16.5" style="2"/>
-    <col min="45" max="49" width="16.83203125" style="2" customWidth="1"/>
-    <col min="50" max="16384" width="16.5" style="2"/>
+    <col min="2" max="2" width="25.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="24"/>
+    <col min="7" max="7" width="16.44140625" style="4"/>
+    <col min="9" max="9" width="16.44140625" style="5"/>
+    <col min="14" max="14" width="25.77734375" customWidth="1"/>
+    <col min="15" max="15" width="25.77734375" style="61" customWidth="1"/>
+    <col min="16" max="16" width="22.109375" customWidth="1"/>
+    <col min="17" max="21" width="16.44140625" customWidth="1"/>
+    <col min="22" max="22" width="16.44140625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="16.44140625" style="36" customWidth="1"/>
+    <col min="24" max="29" width="16.44140625" style="2" customWidth="1"/>
+    <col min="30" max="30" width="16.44140625" style="36" customWidth="1"/>
+    <col min="31" max="37" width="16.44140625" style="2" customWidth="1"/>
+    <col min="38" max="44" width="16.44140625" style="2"/>
+    <col min="45" max="49" width="16.77734375" style="2" customWidth="1"/>
+    <col min="50" max="16384" width="16.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="3" customFormat="1" ht="16">
+    <row r="1" spans="1:52" s="3" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
@@ -8898,19 +8906,19 @@
       <selection pane="bottomRight" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="29.33203125" style="61" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="61"/>
-    <col min="4" max="4" width="16.5" style="26"/>
-    <col min="5" max="5" width="17.5" style="26" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="61"/>
+    <col min="4" max="4" width="16.44140625" style="26"/>
+    <col min="5" max="5" width="17.44140625" style="26" customWidth="1"/>
     <col min="6" max="7" width="24" style="61" customWidth="1"/>
-    <col min="8" max="8" width="22.5" style="20" customWidth="1"/>
+    <col min="8" max="8" width="22.44140625" style="20" customWidth="1"/>
     <col min="9" max="9" width="23.33203125" style="61" customWidth="1"/>
     <col min="10" max="10" width="24" style="61" customWidth="1"/>
     <col min="11" max="11" width="19.33203125" style="61" customWidth="1"/>
-    <col min="12" max="12" width="21.5" style="61" customWidth="1"/>
+    <col min="12" max="12" width="21.44140625" style="61" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -10935,17 +10943,17 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" style="34" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="21.6640625" style="51" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" customWidth="1"/>
     <col min="8" max="8" width="87.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" thickBot="1">
+    <row r="1" spans="1:6" ht="15" thickBot="1">
       <c r="A1" s="38" t="s">
         <v>12</v>
       </c>
@@ -10965,7 +10973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16">
+    <row r="2" spans="1:6">
       <c r="A2" s="40" t="s">
         <v>13</v>
       </c>
@@ -10985,7 +10993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16">
+    <row r="3" spans="1:6">
       <c r="A3" s="40" t="s">
         <v>13</v>
       </c>
@@ -11005,7 +11013,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="32">
+    <row r="4" spans="1:6" ht="43.2">
       <c r="A4" s="40" t="s">
         <v>13</v>
       </c>
@@ -11025,7 +11033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="32">
+    <row r="5" spans="1:6" ht="28.8">
       <c r="A5" s="40" t="s">
         <v>13</v>
       </c>
@@ -11045,7 +11053,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="48">
+    <row r="6" spans="1:6" ht="43.2">
       <c r="A6" s="40" t="s">
         <v>13</v>
       </c>
@@ -11065,7 +11073,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16">
+    <row r="7" spans="1:6">
       <c r="A7" s="40" t="s">
         <v>13</v>
       </c>
@@ -11085,7 +11093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16">
+    <row r="8" spans="1:6">
       <c r="A8" s="40" t="s">
         <v>13</v>
       </c>
@@ -11105,7 +11113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="32">
+    <row r="9" spans="1:6" ht="28.8">
       <c r="A9" s="40" t="s">
         <v>13</v>
       </c>
@@ -11125,7 +11133,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16">
+    <row r="10" spans="1:6">
       <c r="A10" s="40" t="s">
         <v>13</v>
       </c>
@@ -11145,7 +11153,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16">
+    <row r="11" spans="1:6">
       <c r="A11" s="40" t="s">
         <v>13</v>
       </c>
@@ -11165,7 +11173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16">
+    <row r="12" spans="1:6">
       <c r="A12" s="40" t="s">
         <v>13</v>
       </c>
@@ -11185,7 +11193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16">
+    <row r="13" spans="1:6">
       <c r="A13" s="40" t="s">
         <v>13</v>
       </c>
@@ -11205,7 +11213,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="32">
+    <row r="14" spans="1:6" ht="28.8">
       <c r="A14" s="40" t="s">
         <v>13</v>
       </c>
@@ -11225,7 +11233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16">
+    <row r="15" spans="1:6">
       <c r="A15" s="40" t="s">
         <v>13</v>
       </c>
@@ -11285,7 +11293,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="32">
+    <row r="18" spans="1:6" ht="28.8">
       <c r="A18" s="31" t="s">
         <v>15</v>
       </c>
@@ -11305,7 +11313,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="32">
+    <row r="19" spans="1:6" ht="28.8">
       <c r="A19" s="31" t="s">
         <v>15</v>
       </c>
@@ -11325,7 +11333,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="32">
+    <row r="20" spans="1:6" ht="28.8">
       <c r="A20" s="31" t="s">
         <v>15</v>
       </c>
@@ -11345,7 +11353,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="32">
+    <row r="21" spans="1:6" ht="28.8">
       <c r="A21" s="31" t="s">
         <v>15</v>
       </c>
@@ -11365,7 +11373,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="32">
+    <row r="22" spans="1:6" ht="28.8">
       <c r="A22" s="31" t="s">
         <v>15</v>
       </c>
@@ -11385,7 +11393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="32">
+    <row r="23" spans="1:6" ht="28.8">
       <c r="A23" s="31" t="s">
         <v>15</v>
       </c>
@@ -11405,7 +11413,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="48">
+    <row r="24" spans="1:6" ht="43.2">
       <c r="A24" s="31" t="s">
         <v>15</v>
       </c>
@@ -11425,7 +11433,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="32">
+    <row r="25" spans="1:6" ht="28.8">
       <c r="A25" s="31" t="s">
         <v>15</v>
       </c>
@@ -11445,7 +11453,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="32">
+    <row r="26" spans="1:6" ht="28.8">
       <c r="A26" s="31" t="s">
         <v>15</v>
       </c>
@@ -11465,7 +11473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="32">
+    <row r="27" spans="1:6" ht="28.8">
       <c r="A27" s="31" t="s">
         <v>15</v>
       </c>
@@ -11485,7 +11493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="32">
+    <row r="28" spans="1:6" ht="28.8">
       <c r="A28" s="31" t="s">
         <v>15</v>
       </c>
@@ -11505,7 +11513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="32">
+    <row r="29" spans="1:6" ht="28.8">
       <c r="A29" s="31" t="s">
         <v>15</v>
       </c>
@@ -11525,7 +11533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="32">
+    <row r="30" spans="1:6" ht="28.8">
       <c r="A30" s="31" t="s">
         <v>15</v>
       </c>
@@ -11545,7 +11553,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="48">
+    <row r="31" spans="1:6" ht="43.2">
       <c r="A31" s="31" t="s">
         <v>15</v>
       </c>
@@ -11565,7 +11573,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="32">
+    <row r="32" spans="1:6" ht="28.8">
       <c r="A32" s="31" t="s">
         <v>15</v>
       </c>
@@ -11585,7 +11593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="32">
+    <row r="33" spans="1:6" ht="28.8">
       <c r="A33" s="31" t="s">
         <v>15</v>
       </c>
@@ -11605,7 +11613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="32">
+    <row r="34" spans="1:6" ht="28.8">
       <c r="A34" s="31" t="s">
         <v>15</v>
       </c>
@@ -11625,7 +11633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="32">
+    <row r="35" spans="1:6" ht="28.8">
       <c r="A35" s="31" t="s">
         <v>15</v>
       </c>
@@ -11645,7 +11653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="32">
+    <row r="36" spans="1:6" ht="28.8">
       <c r="A36" s="31" t="s">
         <v>15</v>
       </c>
@@ -11665,7 +11673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="32">
+    <row r="37" spans="1:6" ht="28.8">
       <c r="A37" s="31" t="s">
         <v>15</v>
       </c>
@@ -11685,7 +11693,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="48">
+    <row r="38" spans="1:6" ht="43.2">
       <c r="A38" s="31" t="s">
         <v>15</v>
       </c>
@@ -11705,7 +11713,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="32">
+    <row r="39" spans="1:6" ht="28.8">
       <c r="A39" s="31" t="s">
         <v>15</v>
       </c>
@@ -11725,7 +11733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="32">
+    <row r="40" spans="1:6" ht="28.8">
       <c r="A40" s="31" t="s">
         <v>15</v>
       </c>
@@ -11745,7 +11753,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="32">
+    <row r="41" spans="1:6" ht="28.8">
       <c r="A41" s="31" t="s">
         <v>15</v>
       </c>
@@ -11765,7 +11773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="32">
+    <row r="42" spans="1:6" ht="28.8">
       <c r="A42" s="31" t="s">
         <v>15</v>
       </c>
@@ -11785,7 +11793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="32">
+    <row r="43" spans="1:6" ht="28.8">
       <c r="A43" s="31" t="s">
         <v>15</v>
       </c>
@@ -11805,7 +11813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="32">
+    <row r="44" spans="1:6" ht="28.8">
       <c r="A44" s="31" t="s">
         <v>15</v>
       </c>
@@ -11825,7 +11833,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="48">
+    <row r="45" spans="1:6" ht="43.2">
       <c r="A45" s="31" t="s">
         <v>15</v>
       </c>
@@ -11845,7 +11853,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="32">
+    <row r="46" spans="1:6" ht="28.8">
       <c r="A46" s="50" t="s">
         <v>75</v>
       </c>
@@ -11865,7 +11873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="32">
+    <row r="47" spans="1:6" ht="28.8">
       <c r="A47" s="50" t="s">
         <v>75</v>
       </c>
@@ -11885,7 +11893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="32">
+    <row r="48" spans="1:6" ht="28.8">
       <c r="A48" s="50" t="s">
         <v>75</v>
       </c>
@@ -11905,7 +11913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="32">
+    <row r="49" spans="1:6" ht="28.8">
       <c r="A49" s="50" t="s">
         <v>75</v>
       </c>
@@ -11925,7 +11933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="32">
+    <row r="50" spans="1:6" ht="28.8">
       <c r="A50" s="50" t="s">
         <v>75</v>
       </c>
@@ -11945,7 +11953,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="32">
+    <row r="51" spans="1:6" ht="28.8">
       <c r="A51" s="44" t="s">
         <v>14</v>
       </c>
@@ -11965,7 +11973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="48">
+    <row r="52" spans="1:6" ht="43.2">
       <c r="A52" s="44" t="s">
         <v>14</v>
       </c>
@@ -11985,7 +11993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="16">
+    <row r="53" spans="1:6">
       <c r="A53" s="44" t="s">
         <v>14</v>
       </c>
@@ -12005,7 +12013,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="16">
+    <row r="54" spans="1:6">
       <c r="A54" s="44" t="s">
         <v>14</v>
       </c>
@@ -12025,7 +12033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="80">
+    <row r="55" spans="1:6" ht="72">
       <c r="A55" s="44" t="s">
         <v>14</v>
       </c>
@@ -12045,7 +12053,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="64">
+    <row r="56" spans="1:6" ht="72">
       <c r="A56" s="44" t="s">
         <v>14</v>
       </c>
@@ -12065,7 +12073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="16">
+    <row r="57" spans="1:6">
       <c r="A57" s="44" t="s">
         <v>14</v>
       </c>
@@ -12085,7 +12093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="32">
+    <row r="58" spans="1:6" ht="28.8">
       <c r="A58" s="44" t="s">
         <v>14</v>
       </c>
@@ -12105,7 +12113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="48">
+    <row r="59" spans="1:6" ht="43.2">
       <c r="A59" s="45" t="s">
         <v>103</v>
       </c>
@@ -12139,16 +12147,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F8BFE4-8461-B541-8467-258963D3527B}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E34" sqref="E34:E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="40.83203125" customWidth="1"/>
+    <col min="1" max="1" width="40.77734375" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="61" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="61" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12183,7 +12191,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>178650</v>
+        <v>179353</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12201,7 +12209,7 @@
       </c>
       <c r="E3" s="61">
         <f t="shared" ref="E3:E44" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
-        <v>126908</v>
+        <v>105677</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -12219,7 +12227,7 @@
       </c>
       <c r="E4" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>175844</v>
+        <v>180002</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -12237,7 +12245,7 @@
       </c>
       <c r="E5" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>244845</v>
+        <v>181125</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -12255,7 +12263,7 @@
       </c>
       <c r="E6" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>126020</v>
+        <v>110142</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -12273,7 +12281,7 @@
       </c>
       <c r="E7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>103176</v>
+        <v>37775</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -12291,7 +12299,7 @@
       </c>
       <c r="E8" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>167980</v>
+        <v>125089</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -12309,7 +12317,7 @@
       </c>
       <c r="E9" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>245505</v>
+        <v>192445</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -12327,7 +12335,7 @@
       </c>
       <c r="E10" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>216265</v>
+        <v>192964</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -12345,7 +12353,7 @@
       </c>
       <c r="E11" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>173275</v>
+        <v>169628</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -12363,7 +12371,7 @@
       </c>
       <c r="E12" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>67366</v>
+        <v>189709</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -12381,7 +12389,7 @@
       </c>
       <c r="E13" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>120343</v>
+        <v>74760</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -12399,7 +12407,7 @@
       </c>
       <c r="E14" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>70900</v>
+        <v>92367</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -12417,7 +12425,7 @@
       </c>
       <c r="E15" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>122450</v>
+        <v>215631</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -12435,7 +12443,7 @@
       </c>
       <c r="E16" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>235297</v>
+        <v>117852</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -12453,7 +12461,7 @@
       </c>
       <c r="E17" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>84691</v>
+        <v>221092</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -12471,7 +12479,7 @@
       </c>
       <c r="E18" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>206841</v>
+        <v>63533</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -12489,7 +12497,7 @@
       </c>
       <c r="E19" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>77352</v>
+        <v>46333</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -12507,7 +12515,7 @@
       </c>
       <c r="E20" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>138084</v>
+        <v>59182</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -12525,7 +12533,7 @@
       </c>
       <c r="E21" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>99654</v>
+        <v>111757</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -12543,7 +12551,7 @@
       </c>
       <c r="E22" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>186876</v>
+        <v>173130</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -12561,7 +12569,7 @@
       </c>
       <c r="E23" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>222695</v>
+        <v>118519</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -12579,7 +12587,7 @@
       </c>
       <c r="E24" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>152722</v>
+        <v>244771</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -12597,7 +12605,7 @@
       </c>
       <c r="E25" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>118091</v>
+        <v>86206</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -12615,7 +12623,7 @@
       </c>
       <c r="E26" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>60678</v>
+        <v>191525</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -12633,7 +12641,7 @@
       </c>
       <c r="E27" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>224757</v>
+        <v>222771</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -12651,7 +12659,7 @@
       </c>
       <c r="E28" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>191542</v>
+        <v>78428</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -12669,7 +12677,7 @@
       </c>
       <c r="E29" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>191539</v>
+        <v>180926</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -12687,7 +12695,7 @@
       </c>
       <c r="E30" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>104513</v>
+        <v>161497</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -12705,7 +12713,7 @@
       </c>
       <c r="E31" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>245280</v>
+        <v>126039</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -12723,7 +12731,7 @@
       </c>
       <c r="E32" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>174558</v>
+        <v>226403</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -12741,7 +12749,7 @@
       </c>
       <c r="E33" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>126189</v>
+        <v>59641</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -12759,7 +12767,7 @@
       </c>
       <c r="E34" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>123996</v>
+        <v>209763</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -12777,7 +12785,7 @@
       </c>
       <c r="E35" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>138805</v>
+        <v>164605</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -12795,7 +12803,7 @@
       </c>
       <c r="E36" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>227679</v>
+        <v>93798</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -12813,7 +12821,7 @@
       </c>
       <c r="E37" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>198758</v>
+        <v>230985</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -12831,7 +12839,7 @@
       </c>
       <c r="E38" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>102749</v>
+        <v>125142</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -12849,7 +12857,7 @@
       </c>
       <c r="E39" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>38693</v>
+        <v>213931</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -12867,7 +12875,7 @@
       </c>
       <c r="E40" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>195002</v>
+        <v>111727</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -12885,7 +12893,7 @@
       </c>
       <c r="E41" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>204355</v>
+        <v>231965</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -12903,7 +12911,7 @@
       </c>
       <c r="E42" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>57497</v>
+        <v>79656</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -12921,7 +12929,7 @@
       </c>
       <c r="E43" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>120912</v>
+        <v>212205</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -12939,11 +12947,15 @@
       </c>
       <c r="E44" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>79304</v>
+        <v>137063</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000Confidential&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -12961,36 +12973,36 @@
       <selection pane="bottomRight" activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="61"/>
-    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="61"/>
+    <col min="1" max="1" width="16.44140625" style="61"/>
+    <col min="2" max="2" width="25.44140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="61"/>
     <col min="4" max="4" width="8" style="61" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="24"/>
-    <col min="6" max="6" width="16.5" style="61"/>
+    <col min="5" max="5" width="16.44140625" style="24"/>
+    <col min="6" max="6" width="16.44140625" style="61"/>
     <col min="7" max="7" width="10" style="4" customWidth="1"/>
     <col min="8" max="8" width="9" style="61" customWidth="1"/>
     <col min="9" max="9" width="11" style="5" customWidth="1"/>
-    <col min="10" max="13" width="16.5" style="61"/>
+    <col min="10" max="13" width="16.44140625" style="61"/>
     <col min="14" max="14" width="17" style="61" customWidth="1"/>
-    <col min="15" max="15" width="15.5" style="61" customWidth="1"/>
+    <col min="15" max="15" width="15.44140625" style="61" customWidth="1"/>
     <col min="16" max="16" width="16.6640625" style="61" customWidth="1"/>
     <col min="17" max="19" width="0" style="61" hidden="1" customWidth="1"/>
-    <col min="20" max="21" width="16.5" style="61"/>
+    <col min="20" max="21" width="16.44140625" style="61"/>
     <col min="22" max="22" width="0" style="2" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="0" style="36" hidden="1" customWidth="1"/>
     <col min="24" max="29" width="0" style="2" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="0" style="36" hidden="1" customWidth="1"/>
     <col min="31" max="33" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="34" max="36" width="16.5" style="2"/>
+    <col min="34" max="36" width="16.44140625" style="2"/>
     <col min="37" max="44" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="45" max="47" width="16.83203125" style="2" hidden="1" customWidth="1"/>
-    <col min="48" max="49" width="16.83203125" style="2" customWidth="1"/>
-    <col min="50" max="16384" width="16.5" style="2"/>
+    <col min="45" max="47" width="16.77734375" style="2" hidden="1" customWidth="1"/>
+    <col min="48" max="49" width="16.77734375" style="2" customWidth="1"/>
+    <col min="50" max="16384" width="16.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="3" customFormat="1" ht="16">
+    <row r="1" spans="1:52" s="3" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
@@ -17582,20 +17594,20 @@
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="29.33203125" style="61" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="61"/>
-    <col min="4" max="4" width="8.83203125" style="26"/>
-    <col min="5" max="5" width="17.5" style="26" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" style="61"/>
+    <col min="4" max="4" width="8.77734375" style="26"/>
+    <col min="5" max="5" width="17.44140625" style="26" customWidth="1"/>
     <col min="6" max="7" width="24" style="61" customWidth="1"/>
-    <col min="8" max="8" width="22.5" style="20" customWidth="1"/>
+    <col min="8" max="8" width="22.44140625" style="20" customWidth="1"/>
     <col min="9" max="9" width="23.33203125" style="61" customWidth="1"/>
     <col min="10" max="10" width="24" style="61" customWidth="1"/>
     <col min="11" max="11" width="19.33203125" style="61" customWidth="1"/>
-    <col min="12" max="12" width="21.5" style="61" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="61"/>
+    <col min="12" max="12" width="21.44140625" style="61" customWidth="1"/>
+    <col min="13" max="16384" width="8.77734375" style="61"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -18127,15 +18139,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BB6CE2092F7CDA4FBA49881696A89DE0" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b5918a5add965903052caa4f280154e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="020ef37c-4094-40f4-bf82-41b1d62e0e53" xmlns:ns4="40408af7-2a3f-48ae-b560-b937464d5fc3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55d586a85da155bcad137d4f3c4349ba" ns3:_="" ns4:_="">
     <xsd:import namespace="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
@@ -18352,6 +18355,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -18359,14 +18371,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EA39C3-A15D-48B6-A2C6-B0C6753DDE50}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C61229-62A1-4F5F-B8F8-172CE6F3C2F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18381,6 +18385,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EA39C3-A15D-48B6-A2C6-B0C6753DDE50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fix limitation of pint-pandas 0.3
I've somehow fixed this in the MichaelTiemannOSC/pint-pandas branch.  I've submitted an issue to pint-pandas: https://github.com/hgrecco/pint-pandas/issues/167

In the meantime, this is a work-around, with bug fixes also due to fixing some test data typos that were discovered.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data/20220215 ITR Tool Sample Data.xlsx
+++ b/examples/data/20220215 ITR Tool Sample Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/MichaelTiemannOSC/ITR/examples/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/MichaelTiemannOSC/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEB138B-A96E-9D4E-AD3A-A3B243E6AF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8329844-CA0E-3E4B-97FA-2E89E92EB3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6620" yWindow="11420" windowWidth="23260" windowHeight="12580" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38420" yWindow="8820" windowWidth="32480" windowHeight="12580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -3364,11 +3364,11 @@
   </sheetPr>
   <dimension ref="A1:AZ52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -3683,7 +3683,7 @@
         <v>83985.94</v>
       </c>
       <c r="AV2">
-        <v>759043.55</v>
+        <v>75043.55</v>
       </c>
       <c r="AW2">
         <v>75271.521999999997</v>
@@ -8079,7 +8079,7 @@
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
@@ -11331,7 +11331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F8BFE4-8461-B541-8467-258963D3527B}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -12100,6 +12100,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BB6CE2092F7CDA4FBA49881696A89DE0" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b5918a5add965903052caa4f280154e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="020ef37c-4094-40f4-bf82-41b1d62e0e53" xmlns:ns4="40408af7-2a3f-48ae-b560-b937464d5fc3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55d586a85da155bcad137d4f3c4349ba" ns3:_="" ns4:_="">
     <xsd:import namespace="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
@@ -12316,15 +12325,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -12332,6 +12332,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EA39C3-A15D-48B6-A2C6-B0C6753DDE50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C61229-62A1-4F5F-B8F8-172CE6F3C2F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12346,14 +12354,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EA39C3-A15D-48B6-A2C6-B0C6753DDE50}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>